<commit_message>
Small Fixes, docs updated
Closes #6
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECC240-9DEA-4496-A80B-954750B9DA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC86949C-0136-4781-A888-331CCCBF31B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-8085" yWindow="-18150" windowWidth="22110" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1101,11 +1101,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1125,42 +1127,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1170,8 +1136,47 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1200,32 +1205,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -3592,8 +3592,8 @@
   </sheetPr>
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X34" sqref="X34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3634,246 +3634,246 @@
   <sheetData>
     <row r="1" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="200" t="s">
+      <c r="B2" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="201"/>
-      <c r="D2" s="202"/>
-      <c r="E2" s="196" t="s">
+      <c r="C2" s="204"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="186" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="197"/>
-      <c r="G2" s="197"/>
-      <c r="H2" s="197"/>
-      <c r="I2" s="197"/>
-      <c r="J2" s="197"/>
-      <c r="K2" s="197"/>
-      <c r="L2" s="197"/>
-      <c r="M2" s="197"/>
-      <c r="N2" s="197"/>
-      <c r="O2" s="197"/>
-      <c r="P2" s="197"/>
-      <c r="Q2" s="197"/>
-      <c r="R2" s="197"/>
-      <c r="S2" s="197"/>
-      <c r="T2" s="198"/>
-      <c r="U2" s="196" t="s">
+      <c r="F2" s="187"/>
+      <c r="G2" s="187"/>
+      <c r="H2" s="187"/>
+      <c r="I2" s="187"/>
+      <c r="J2" s="187"/>
+      <c r="K2" s="187"/>
+      <c r="L2" s="187"/>
+      <c r="M2" s="187"/>
+      <c r="N2" s="187"/>
+      <c r="O2" s="187"/>
+      <c r="P2" s="187"/>
+      <c r="Q2" s="187"/>
+      <c r="R2" s="187"/>
+      <c r="S2" s="187"/>
+      <c r="T2" s="188"/>
+      <c r="U2" s="186" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="197"/>
-      <c r="W2" s="197"/>
-      <c r="X2" s="197"/>
-      <c r="Y2" s="197"/>
-      <c r="Z2" s="197"/>
-      <c r="AA2" s="197"/>
-      <c r="AB2" s="197"/>
-      <c r="AC2" s="197"/>
-      <c r="AD2" s="197"/>
-      <c r="AE2" s="197"/>
-      <c r="AF2" s="197"/>
-      <c r="AG2" s="197"/>
-      <c r="AH2" s="197"/>
-      <c r="AI2" s="197"/>
-      <c r="AJ2" s="197"/>
-      <c r="AK2" s="197"/>
-      <c r="AL2" s="197"/>
-      <c r="AM2" s="197"/>
-      <c r="AN2" s="198"/>
-      <c r="AO2" s="196" t="s">
+      <c r="V2" s="187"/>
+      <c r="W2" s="187"/>
+      <c r="X2" s="187"/>
+      <c r="Y2" s="187"/>
+      <c r="Z2" s="187"/>
+      <c r="AA2" s="187"/>
+      <c r="AB2" s="187"/>
+      <c r="AC2" s="187"/>
+      <c r="AD2" s="187"/>
+      <c r="AE2" s="187"/>
+      <c r="AF2" s="187"/>
+      <c r="AG2" s="187"/>
+      <c r="AH2" s="187"/>
+      <c r="AI2" s="187"/>
+      <c r="AJ2" s="187"/>
+      <c r="AK2" s="187"/>
+      <c r="AL2" s="187"/>
+      <c r="AM2" s="187"/>
+      <c r="AN2" s="188"/>
+      <c r="AO2" s="186" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" s="197"/>
-      <c r="AQ2" s="197"/>
-      <c r="AR2" s="197"/>
-      <c r="AS2" s="197"/>
-      <c r="AT2" s="197"/>
-      <c r="AU2" s="197"/>
-      <c r="AV2" s="197"/>
-      <c r="AW2" s="197"/>
-      <c r="AX2" s="197"/>
-      <c r="AY2" s="197"/>
-      <c r="AZ2" s="197"/>
-      <c r="BA2" s="197"/>
-      <c r="BB2" s="197"/>
-      <c r="BC2" s="197"/>
-      <c r="BD2" s="197"/>
-      <c r="BE2" s="197"/>
-      <c r="BF2" s="197"/>
-      <c r="BG2" s="197"/>
-      <c r="BH2" s="198"/>
-      <c r="BI2" s="196" t="s">
+      <c r="AP2" s="187"/>
+      <c r="AQ2" s="187"/>
+      <c r="AR2" s="187"/>
+      <c r="AS2" s="187"/>
+      <c r="AT2" s="187"/>
+      <c r="AU2" s="187"/>
+      <c r="AV2" s="187"/>
+      <c r="AW2" s="187"/>
+      <c r="AX2" s="187"/>
+      <c r="AY2" s="187"/>
+      <c r="AZ2" s="187"/>
+      <c r="BA2" s="187"/>
+      <c r="BB2" s="187"/>
+      <c r="BC2" s="187"/>
+      <c r="BD2" s="187"/>
+      <c r="BE2" s="187"/>
+      <c r="BF2" s="187"/>
+      <c r="BG2" s="187"/>
+      <c r="BH2" s="188"/>
+      <c r="BI2" s="186" t="s">
         <v>63</v>
       </c>
-      <c r="BJ2" s="197"/>
-      <c r="BK2" s="197"/>
-      <c r="BL2" s="198"/>
+      <c r="BJ2" s="187"/>
+      <c r="BK2" s="187"/>
+      <c r="BL2" s="188"/>
     </row>
     <row r="3" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="203" t="s">
+      <c r="B3" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="204"/>
-      <c r="D3" s="207" t="s">
+      <c r="C3" s="207"/>
+      <c r="D3" s="210" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="178" t="s">
+      <c r="E3" s="180" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="180"/>
-      <c r="I3" s="178" t="s">
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="182"/>
+      <c r="I3" s="180" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="179"/>
-      <c r="K3" s="179"/>
-      <c r="L3" s="180"/>
-      <c r="M3" s="178" t="s">
+      <c r="J3" s="181"/>
+      <c r="K3" s="181"/>
+      <c r="L3" s="182"/>
+      <c r="M3" s="180" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="179"/>
-      <c r="O3" s="179"/>
-      <c r="P3" s="180"/>
-      <c r="Q3" s="178" t="s">
+      <c r="N3" s="181"/>
+      <c r="O3" s="181"/>
+      <c r="P3" s="182"/>
+      <c r="Q3" s="180" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="179"/>
-      <c r="S3" s="179"/>
-      <c r="T3" s="180"/>
-      <c r="U3" s="178" t="s">
+      <c r="R3" s="181"/>
+      <c r="S3" s="181"/>
+      <c r="T3" s="182"/>
+      <c r="U3" s="180" t="s">
         <v>49</v>
       </c>
-      <c r="V3" s="179"/>
-      <c r="W3" s="179"/>
-      <c r="X3" s="180"/>
-      <c r="Y3" s="178" t="s">
+      <c r="V3" s="181"/>
+      <c r="W3" s="181"/>
+      <c r="X3" s="182"/>
+      <c r="Y3" s="180" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" s="179"/>
-      <c r="AA3" s="179"/>
-      <c r="AB3" s="180"/>
-      <c r="AC3" s="178" t="s">
+      <c r="Z3" s="181"/>
+      <c r="AA3" s="181"/>
+      <c r="AB3" s="182"/>
+      <c r="AC3" s="180" t="s">
         <v>51</v>
       </c>
-      <c r="AD3" s="179"/>
-      <c r="AE3" s="179"/>
-      <c r="AF3" s="180"/>
-      <c r="AG3" s="178" t="s">
+      <c r="AD3" s="181"/>
+      <c r="AE3" s="181"/>
+      <c r="AF3" s="182"/>
+      <c r="AG3" s="180" t="s">
         <v>52</v>
       </c>
-      <c r="AH3" s="179"/>
-      <c r="AI3" s="179"/>
-      <c r="AJ3" s="180"/>
-      <c r="AK3" s="178" t="s">
+      <c r="AH3" s="181"/>
+      <c r="AI3" s="181"/>
+      <c r="AJ3" s="182"/>
+      <c r="AK3" s="180" t="s">
         <v>53</v>
       </c>
-      <c r="AL3" s="179"/>
-      <c r="AM3" s="179"/>
-      <c r="AN3" s="180"/>
-      <c r="AO3" s="178" t="s">
+      <c r="AL3" s="181"/>
+      <c r="AM3" s="181"/>
+      <c r="AN3" s="182"/>
+      <c r="AO3" s="180" t="s">
         <v>54</v>
       </c>
-      <c r="AP3" s="179"/>
-      <c r="AQ3" s="179"/>
-      <c r="AR3" s="180"/>
-      <c r="AS3" s="178" t="s">
+      <c r="AP3" s="181"/>
+      <c r="AQ3" s="181"/>
+      <c r="AR3" s="182"/>
+      <c r="AS3" s="180" t="s">
         <v>55</v>
       </c>
-      <c r="AT3" s="179"/>
-      <c r="AU3" s="179"/>
-      <c r="AV3" s="180"/>
-      <c r="AW3" s="178" t="s">
+      <c r="AT3" s="181"/>
+      <c r="AU3" s="181"/>
+      <c r="AV3" s="182"/>
+      <c r="AW3" s="180" t="s">
         <v>56</v>
       </c>
-      <c r="AX3" s="179"/>
-      <c r="AY3" s="179"/>
-      <c r="AZ3" s="180"/>
-      <c r="BA3" s="178" t="s">
+      <c r="AX3" s="181"/>
+      <c r="AY3" s="181"/>
+      <c r="AZ3" s="182"/>
+      <c r="BA3" s="180" t="s">
         <v>57</v>
       </c>
-      <c r="BB3" s="179"/>
-      <c r="BC3" s="179"/>
-      <c r="BD3" s="180"/>
-      <c r="BE3" s="178" t="s">
+      <c r="BB3" s="181"/>
+      <c r="BC3" s="181"/>
+      <c r="BD3" s="182"/>
+      <c r="BE3" s="180" t="s">
         <v>58</v>
       </c>
-      <c r="BF3" s="179"/>
-      <c r="BG3" s="179"/>
-      <c r="BH3" s="180"/>
-      <c r="BI3" s="178" t="s">
+      <c r="BF3" s="181"/>
+      <c r="BG3" s="181"/>
+      <c r="BH3" s="182"/>
+      <c r="BI3" s="180" t="s">
         <v>59</v>
       </c>
-      <c r="BJ3" s="179"/>
-      <c r="BK3" s="179"/>
-      <c r="BL3" s="180"/>
+      <c r="BJ3" s="181"/>
+      <c r="BK3" s="181"/>
+      <c r="BL3" s="182"/>
     </row>
     <row r="4" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="205"/>
-      <c r="C4" s="206"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="182"/>
-      <c r="G4" s="182"/>
-      <c r="H4" s="183"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="182"/>
-      <c r="K4" s="182"/>
-      <c r="L4" s="183"/>
-      <c r="M4" s="181"/>
-      <c r="N4" s="182"/>
-      <c r="O4" s="182"/>
-      <c r="P4" s="183"/>
-      <c r="Q4" s="181"/>
-      <c r="R4" s="182"/>
-      <c r="S4" s="182"/>
-      <c r="T4" s="183"/>
-      <c r="U4" s="181"/>
-      <c r="V4" s="182"/>
-      <c r="W4" s="182"/>
-      <c r="X4" s="183"/>
-      <c r="Y4" s="181"/>
-      <c r="Z4" s="182"/>
-      <c r="AA4" s="182"/>
-      <c r="AB4" s="183"/>
-      <c r="AC4" s="181"/>
-      <c r="AD4" s="182"/>
-      <c r="AE4" s="182"/>
-      <c r="AF4" s="183"/>
-      <c r="AG4" s="181"/>
-      <c r="AH4" s="182"/>
-      <c r="AI4" s="182"/>
-      <c r="AJ4" s="183"/>
-      <c r="AK4" s="181"/>
-      <c r="AL4" s="182"/>
-      <c r="AM4" s="182"/>
-      <c r="AN4" s="183"/>
-      <c r="AO4" s="181"/>
-      <c r="AP4" s="182"/>
-      <c r="AQ4" s="182"/>
-      <c r="AR4" s="183"/>
-      <c r="AS4" s="181"/>
-      <c r="AT4" s="182"/>
-      <c r="AU4" s="182"/>
-      <c r="AV4" s="183"/>
-      <c r="AW4" s="181"/>
-      <c r="AX4" s="182"/>
-      <c r="AY4" s="182"/>
-      <c r="AZ4" s="183"/>
-      <c r="BA4" s="181"/>
-      <c r="BB4" s="182"/>
-      <c r="BC4" s="182"/>
-      <c r="BD4" s="183"/>
-      <c r="BE4" s="181"/>
-      <c r="BF4" s="182"/>
-      <c r="BG4" s="182"/>
-      <c r="BH4" s="183"/>
-      <c r="BI4" s="181"/>
-      <c r="BJ4" s="182"/>
-      <c r="BK4" s="182"/>
-      <c r="BL4" s="183"/>
+      <c r="B4" s="208"/>
+      <c r="C4" s="209"/>
+      <c r="D4" s="211"/>
+      <c r="E4" s="183"/>
+      <c r="F4" s="184"/>
+      <c r="G4" s="184"/>
+      <c r="H4" s="185"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="184"/>
+      <c r="K4" s="184"/>
+      <c r="L4" s="185"/>
+      <c r="M4" s="183"/>
+      <c r="N4" s="184"/>
+      <c r="O4" s="184"/>
+      <c r="P4" s="185"/>
+      <c r="Q4" s="183"/>
+      <c r="R4" s="184"/>
+      <c r="S4" s="184"/>
+      <c r="T4" s="185"/>
+      <c r="U4" s="183"/>
+      <c r="V4" s="184"/>
+      <c r="W4" s="184"/>
+      <c r="X4" s="185"/>
+      <c r="Y4" s="183"/>
+      <c r="Z4" s="184"/>
+      <c r="AA4" s="184"/>
+      <c r="AB4" s="185"/>
+      <c r="AC4" s="183"/>
+      <c r="AD4" s="184"/>
+      <c r="AE4" s="184"/>
+      <c r="AF4" s="185"/>
+      <c r="AG4" s="183"/>
+      <c r="AH4" s="184"/>
+      <c r="AI4" s="184"/>
+      <c r="AJ4" s="185"/>
+      <c r="AK4" s="183"/>
+      <c r="AL4" s="184"/>
+      <c r="AM4" s="184"/>
+      <c r="AN4" s="185"/>
+      <c r="AO4" s="183"/>
+      <c r="AP4" s="184"/>
+      <c r="AQ4" s="184"/>
+      <c r="AR4" s="185"/>
+      <c r="AS4" s="183"/>
+      <c r="AT4" s="184"/>
+      <c r="AU4" s="184"/>
+      <c r="AV4" s="185"/>
+      <c r="AW4" s="183"/>
+      <c r="AX4" s="184"/>
+      <c r="AY4" s="184"/>
+      <c r="AZ4" s="185"/>
+      <c r="BA4" s="183"/>
+      <c r="BB4" s="184"/>
+      <c r="BC4" s="184"/>
+      <c r="BD4" s="185"/>
+      <c r="BE4" s="183"/>
+      <c r="BF4" s="184"/>
+      <c r="BG4" s="184"/>
+      <c r="BH4" s="185"/>
+      <c r="BI4" s="183"/>
+      <c r="BJ4" s="184"/>
+      <c r="BK4" s="184"/>
+      <c r="BL4" s="185"/>
     </row>
     <row r="5" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="197" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="43" t="s">
@@ -3945,7 +3945,7 @@
       <c r="BL5" s="22"/>
     </row>
     <row r="6" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B6" s="199"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4015,7 +4015,7 @@
       <c r="BL6" s="25"/>
     </row>
     <row r="7" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B7" s="176" t="s">
+      <c r="B7" s="195" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4089,7 +4089,7 @@
       <c r="BL7" s="25"/>
     </row>
     <row r="8" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B8" s="177"/>
+      <c r="B8" s="196"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -4170,7 +4170,7 @@
       <c r="BV8" s="90"/>
     </row>
     <row r="9" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B9" s="176" t="s">
+      <c r="B9" s="195" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4244,7 +4244,7 @@
       <c r="BL9" s="25"/>
     </row>
     <row r="10" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B10" s="177"/>
+      <c r="B10" s="196"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="BV10" s="92"/>
     </row>
     <row r="11" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="176" t="s">
+      <c r="B11" s="195" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4398,7 +4398,7 @@
       <c r="BL11" s="25"/>
     </row>
     <row r="12" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="193"/>
+      <c r="B12" s="202"/>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
@@ -4470,7 +4470,7 @@
       <c r="BL12" s="31"/>
     </row>
     <row r="13" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="197" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="43" t="s">
@@ -4542,7 +4542,7 @@
       <c r="BL13" s="52"/>
     </row>
     <row r="14" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B14" s="199"/>
+      <c r="B14" s="201"/>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4612,7 +4612,7 @@
       <c r="BL14" s="25"/>
     </row>
     <row r="15" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B15" s="176" t="s">
+      <c r="B15" s="195" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -4688,7 +4688,7 @@
       <c r="BL15" s="25"/>
     </row>
     <row r="16" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B16" s="177"/>
+      <c r="B16" s="196"/>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
@@ -4762,7 +4762,7 @@
       <c r="BL16" s="25"/>
     </row>
     <row r="17" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B17" s="176" t="s">
+      <c r="B17" s="195" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -4838,7 +4838,7 @@
       <c r="BL17" s="25"/>
     </row>
     <row r="18" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B18" s="177"/>
+      <c r="B18" s="196"/>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4912,7 +4912,7 @@
       <c r="BL18" s="25"/>
     </row>
     <row r="19" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B19" s="176" t="s">
+      <c r="B19" s="195" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -4986,7 +4986,7 @@
       <c r="BL19" s="25"/>
     </row>
     <row r="20" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B20" s="177"/>
+      <c r="B20" s="196"/>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -5058,7 +5058,7 @@
       <c r="BL20" s="25"/>
     </row>
     <row r="21" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="195" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5132,7 +5132,7 @@
       <c r="BL21" s="25"/>
     </row>
     <row r="22" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B22" s="177"/>
+      <c r="B22" s="196"/>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
@@ -5204,7 +5204,7 @@
       <c r="BL22" s="25"/>
     </row>
     <row r="23" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="195" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5278,7 +5278,7 @@
       <c r="BL23" s="25"/>
     </row>
     <row r="24" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="193"/>
+      <c r="B24" s="202"/>
       <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
@@ -5350,7 +5350,7 @@
       <c r="BL24" s="31"/>
     </row>
     <row r="25" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B25" s="194" t="s">
+      <c r="B25" s="197" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -5424,7 +5424,7 @@
       <c r="BL25" s="52"/>
     </row>
     <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="195"/>
+      <c r="B26" s="198"/>
       <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
@@ -5496,7 +5496,7 @@
       <c r="BL26" s="31"/>
     </row>
     <row r="27" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B27" s="194" t="s">
+      <c r="B27" s="197" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -5568,13 +5568,13 @@
       <c r="BL27" s="22"/>
     </row>
     <row r="28" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B28" s="199"/>
+      <c r="B28" s="201"/>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>14.25</v>
+        <v>17.25</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -5638,7 +5638,7 @@
       <c r="BL28" s="25"/>
     </row>
     <row r="29" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B29" s="176" t="s">
+      <c r="B29" s="195" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -5714,7 +5714,7 @@
       <c r="BL29" s="25"/>
     </row>
     <row r="30" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B30" s="177"/>
+      <c r="B30" s="196"/>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
@@ -5788,7 +5788,7 @@
       <c r="BL30" s="25"/>
     </row>
     <row r="31" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B31" s="176" t="s">
+      <c r="B31" s="195" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -5864,7 +5864,7 @@
       <c r="BL31" s="25"/>
     </row>
     <row r="32" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B32" s="177"/>
+      <c r="B32" s="196"/>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
@@ -5940,7 +5940,7 @@
       <c r="BL32" s="25"/>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B33" s="176" t="s">
+      <c r="B33" s="195" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -6016,7 +6016,7 @@
       <c r="BL33" s="25"/>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B34" s="177"/>
+      <c r="B34" s="196"/>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
@@ -6043,7 +6043,7 @@
       <c r="U34" s="146">
         <v>2</v>
       </c>
-      <c r="V34" s="217">
+      <c r="V34" s="176">
         <v>1</v>
       </c>
       <c r="W34" s="140">
@@ -6094,7 +6094,7 @@
       <c r="BL34" s="25"/>
     </row>
     <row r="35" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B35" s="176" t="s">
+      <c r="B35" s="195" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -6168,7 +6168,7 @@
       <c r="BL35" s="25"/>
     </row>
     <row r="36" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B36" s="177"/>
+      <c r="B36" s="196"/>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
@@ -6193,7 +6193,7 @@
       <c r="S36" s="69"/>
       <c r="T36" s="70"/>
       <c r="U36" s="32"/>
-      <c r="V36" s="217">
+      <c r="V36" s="176">
         <v>1</v>
       </c>
       <c r="W36" s="140">
@@ -6242,7 +6242,7 @@
       <c r="BL36" s="25"/>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B37" s="176" t="s">
+      <c r="B37" s="195" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -6316,7 +6316,7 @@
       <c r="BL37" s="25"/>
     </row>
     <row r="38" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B38" s="177"/>
+      <c r="B38" s="196"/>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -6388,7 +6388,7 @@
       <c r="BL38" s="25"/>
     </row>
     <row r="39" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B39" s="176" t="s">
+      <c r="B39" s="195" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -6468,13 +6468,13 @@
       <c r="BL39" s="25"/>
     </row>
     <row r="40" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B40" s="177"/>
+      <c r="B40" s="196"/>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="88">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E40" s="71"/>
       <c r="F40" s="69"/>
@@ -6496,8 +6496,12 @@
       <c r="V40" s="91"/>
       <c r="W40" s="16"/>
       <c r="X40" s="17"/>
-      <c r="Y40" s="32"/>
-      <c r="Z40" s="16"/>
+      <c r="Y40" s="32">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="16">
+        <v>1</v>
+      </c>
       <c r="AA40" s="16"/>
       <c r="AB40" s="17"/>
       <c r="AC40" s="85"/>
@@ -6538,7 +6542,7 @@
       <c r="BL40" s="25"/>
     </row>
     <row r="41" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B41" s="176" t="s">
+      <c r="B41" s="195" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -6618,7 +6622,7 @@
       <c r="BL41" s="25"/>
     </row>
     <row r="42" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B42" s="177"/>
+      <c r="B42" s="196"/>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
@@ -6688,7 +6692,7 @@
       <c r="BL42" s="25"/>
     </row>
     <row r="43" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B43" s="176" t="s">
+      <c r="B43" s="195" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6768,7 +6772,7 @@
       <c r="BL43" s="25"/>
     </row>
     <row r="44" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B44" s="177"/>
+      <c r="B44" s="196"/>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
@@ -6838,7 +6842,7 @@
       <c r="BL44" s="25"/>
     </row>
     <row r="45" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B45" s="176" t="s">
+      <c r="B45" s="195" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -6914,7 +6918,7 @@
       <c r="BL45" s="25"/>
     </row>
     <row r="46" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B46" s="177"/>
+      <c r="B46" s="196"/>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
@@ -6984,7 +6988,7 @@
       <c r="BL46" s="25"/>
     </row>
     <row r="47" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B47" s="176" t="s">
+      <c r="B47" s="195" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -7064,7 +7068,7 @@
       <c r="BL47" s="25"/>
     </row>
     <row r="48" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="177"/>
+      <c r="B48" s="196"/>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
@@ -7134,7 +7138,7 @@
       <c r="BL48" s="25"/>
     </row>
     <row r="49" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B49" s="194" t="s">
+      <c r="B49" s="197" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="43" t="s">
@@ -7210,7 +7214,7 @@
       <c r="BL49" s="52"/>
     </row>
     <row r="50" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="195"/>
+      <c r="B50" s="198"/>
       <c r="C50" s="7" t="s">
         <v>3</v>
       </c>
@@ -7280,7 +7284,7 @@
       <c r="BL50" s="31"/>
     </row>
     <row r="51" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B51" s="194" t="s">
+      <c r="B51" s="197" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="43" t="s">
@@ -7356,7 +7360,7 @@
       <c r="BL51" s="52"/>
     </row>
     <row r="52" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="195"/>
+      <c r="B52" s="198"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -7426,7 +7430,7 @@
       <c r="BL52" s="31"/>
     </row>
     <row r="53" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B53" s="194" t="s">
+      <c r="B53" s="197" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="43" t="s">
@@ -7502,7 +7506,7 @@
       <c r="BL53" s="52"/>
     </row>
     <row r="54" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="195"/>
+      <c r="B54" s="198"/>
       <c r="C54" s="7" t="s">
         <v>3</v>
       </c>
@@ -7572,7 +7576,7 @@
       <c r="BL54" s="31"/>
     </row>
     <row r="55" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B55" s="194" t="s">
+      <c r="B55" s="197" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="43" t="s">
@@ -7670,7 +7674,7 @@
       <c r="BL55" s="110"/>
     </row>
     <row r="56" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="195"/>
+      <c r="B56" s="198"/>
       <c r="C56" s="7" t="s">
         <v>3</v>
       </c>
@@ -7750,7 +7754,7 @@
       <c r="BL56" s="31"/>
     </row>
     <row r="57" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B57" s="215" t="s">
+      <c r="B57" s="199" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="54"/>
@@ -7817,7 +7821,7 @@
       <c r="BL57" s="57"/>
     </row>
     <row r="58" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="216"/>
+      <c r="B58" s="200"/>
       <c r="C58" s="59"/>
       <c r="D58" s="60"/>
       <c r="E58" s="63"/>
@@ -7882,11 +7886,11 @@
       <c r="BL58" s="62"/>
     </row>
     <row r="59" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B59" s="209" t="s">
+      <c r="B59" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="210"/>
-      <c r="D59" s="211"/>
+      <c r="C59" s="190"/>
+      <c r="D59" s="191"/>
       <c r="E59" s="144"/>
       <c r="F59" s="145"/>
       <c r="G59" s="172"/>
@@ -7949,9 +7953,9 @@
       <c r="BL59" s="112"/>
     </row>
     <row r="60" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="212"/>
-      <c r="C60" s="213"/>
-      <c r="D60" s="214"/>
+      <c r="B60" s="192"/>
+      <c r="C60" s="193"/>
+      <c r="D60" s="194"/>
       <c r="E60" s="137"/>
       <c r="F60" s="142"/>
       <c r="G60" s="173"/>
@@ -8014,11 +8018,11 @@
       <c r="BL60" s="31"/>
     </row>
     <row r="61" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B61" s="209" t="s">
+      <c r="B61" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="210"/>
-      <c r="D61" s="211"/>
+      <c r="C61" s="190"/>
+      <c r="D61" s="191"/>
       <c r="E61" s="80"/>
       <c r="F61" s="145"/>
       <c r="G61" s="145"/>
@@ -8081,9 +8085,9 @@
       <c r="BL61" s="113"/>
     </row>
     <row r="62" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="212"/>
-      <c r="C62" s="213"/>
-      <c r="D62" s="214"/>
+      <c r="B62" s="192"/>
+      <c r="C62" s="193"/>
+      <c r="D62" s="194"/>
       <c r="E62" s="74"/>
       <c r="F62" s="142"/>
       <c r="G62" s="142"/>
@@ -8146,11 +8150,11 @@
       <c r="BL62" s="31"/>
     </row>
     <row r="63" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B63" s="209" t="s">
+      <c r="B63" s="189" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="210"/>
-      <c r="D63" s="211"/>
+      <c r="C63" s="190"/>
+      <c r="D63" s="191"/>
       <c r="E63" s="80"/>
       <c r="F63" s="78"/>
       <c r="G63" s="78"/>
@@ -8213,9 +8217,9 @@
       <c r="BL63" s="113"/>
     </row>
     <row r="64" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="212"/>
-      <c r="C64" s="213"/>
-      <c r="D64" s="214"/>
+      <c r="B64" s="192"/>
+      <c r="C64" s="193"/>
+      <c r="D64" s="194"/>
       <c r="E64" s="74"/>
       <c r="F64" s="73"/>
       <c r="G64" s="73"/>
@@ -8278,11 +8282,11 @@
       <c r="BL64" s="31"/>
     </row>
     <row r="65" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B65" s="209" t="s">
+      <c r="B65" s="189" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="210"/>
-      <c r="D65" s="211"/>
+      <c r="C65" s="190"/>
+      <c r="D65" s="191"/>
       <c r="E65" s="80"/>
       <c r="F65" s="78"/>
       <c r="G65" s="78"/>
@@ -8345,9 +8349,9 @@
       <c r="BL65" s="113"/>
     </row>
     <row r="66" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="212"/>
-      <c r="C66" s="213"/>
-      <c r="D66" s="214"/>
+      <c r="B66" s="192"/>
+      <c r="C66" s="193"/>
+      <c r="D66" s="194"/>
       <c r="E66" s="74"/>
       <c r="F66" s="73"/>
       <c r="G66" s="73"/>
@@ -8361,11 +8365,11 @@
       <c r="O66" s="30"/>
       <c r="P66" s="31"/>
       <c r="Q66" s="137"/>
-      <c r="R66" s="218"/>
+      <c r="R66" s="177"/>
       <c r="S66" s="142"/>
       <c r="T66" s="164"/>
       <c r="U66" s="137"/>
-      <c r="V66" s="218"/>
+      <c r="V66" s="177"/>
       <c r="W66" s="18"/>
       <c r="X66" s="19"/>
       <c r="Y66" s="35"/>
@@ -8410,11 +8414,11 @@
       <c r="BL66" s="31"/>
     </row>
     <row r="67" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B67" s="209" t="s">
+      <c r="B67" s="189" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="210"/>
-      <c r="D67" s="211"/>
+      <c r="C67" s="190"/>
+      <c r="D67" s="191"/>
       <c r="E67" s="80"/>
       <c r="F67" s="78"/>
       <c r="G67" s="78"/>
@@ -8477,9 +8481,9 @@
       <c r="BL67" s="113"/>
     </row>
     <row r="68" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="212"/>
-      <c r="C68" s="213"/>
-      <c r="D68" s="214"/>
+      <c r="B68" s="192"/>
+      <c r="C68" s="193"/>
+      <c r="D68" s="194"/>
       <c r="E68" s="74"/>
       <c r="F68" s="73"/>
       <c r="G68" s="73"/>
@@ -8542,11 +8546,11 @@
       <c r="BL68" s="31"/>
     </row>
     <row r="69" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B69" s="209" t="s">
+      <c r="B69" s="189" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="210"/>
-      <c r="D69" s="211"/>
+      <c r="C69" s="190"/>
+      <c r="D69" s="191"/>
       <c r="E69" s="80"/>
       <c r="F69" s="78"/>
       <c r="G69" s="78"/>
@@ -8609,9 +8613,9 @@
       <c r="BL69" s="113"/>
     </row>
     <row r="70" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="212"/>
-      <c r="C70" s="213"/>
-      <c r="D70" s="214"/>
+      <c r="B70" s="192"/>
+      <c r="C70" s="193"/>
+      <c r="D70" s="194"/>
       <c r="E70" s="74"/>
       <c r="F70" s="73"/>
       <c r="G70" s="73"/>
@@ -8674,11 +8678,11 @@
       <c r="BL70" s="31"/>
     </row>
     <row r="71" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B71" s="209" t="s">
+      <c r="B71" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="210"/>
-      <c r="D71" s="211"/>
+      <c r="C71" s="190"/>
+      <c r="D71" s="191"/>
       <c r="E71" s="80"/>
       <c r="F71" s="78"/>
       <c r="G71" s="78"/>
@@ -8741,9 +8745,9 @@
       <c r="BL71" s="113"/>
     </row>
     <row r="72" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="212"/>
-      <c r="C72" s="213"/>
-      <c r="D72" s="214"/>
+      <c r="B72" s="192"/>
+      <c r="C72" s="193"/>
+      <c r="D72" s="194"/>
       <c r="E72" s="74"/>
       <c r="F72" s="73"/>
       <c r="G72" s="73"/>
@@ -8824,55 +8828,55 @@
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
-      <c r="E74" s="189" t="s">
+      <c r="E74" s="215" t="s">
         <v>2</v>
       </c>
-      <c r="F74" s="190"/>
-      <c r="G74" s="190"/>
+      <c r="F74" s="216"/>
+      <c r="G74" s="216"/>
       <c r="H74" s="64"/>
-      <c r="I74" s="189" t="s">
+      <c r="I74" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="190"/>
-      <c r="K74" s="190"/>
+      <c r="J74" s="216"/>
+      <c r="K74" s="216"/>
       <c r="L74" s="65"/>
-      <c r="M74" s="191" t="s">
+      <c r="M74" s="217" t="s">
         <v>14</v>
       </c>
-      <c r="N74" s="192"/>
-      <c r="O74" s="192"/>
+      <c r="N74" s="218"/>
+      <c r="O74" s="218"/>
       <c r="P74" s="66"/>
-      <c r="Q74" s="184" t="s">
+      <c r="Q74" s="212" t="s">
         <v>15</v>
       </c>
-      <c r="R74" s="185"/>
-      <c r="S74" s="185"/>
-      <c r="T74" s="185"/>
+      <c r="R74" s="213"/>
+      <c r="S74" s="213"/>
+      <c r="T74" s="213"/>
       <c r="U74" s="67"/>
       <c r="V74" s="135"/>
-      <c r="W74" s="185" t="s">
+      <c r="W74" s="213" t="s">
         <v>28</v>
       </c>
-      <c r="X74" s="185"/>
-      <c r="Y74" s="185"/>
+      <c r="X74" s="213"/>
+      <c r="Y74" s="213"/>
       <c r="Z74" s="68"/>
-      <c r="AA74" s="186" t="s">
+      <c r="AA74" s="178" t="s">
         <v>64</v>
       </c>
-      <c r="AB74" s="187"/>
-      <c r="AC74" s="187"/>
-      <c r="AD74" s="187"/>
-      <c r="AE74" s="187"/>
-      <c r="AF74" s="187"/>
-      <c r="AG74" s="188"/>
-      <c r="AH74" s="186" t="s">
+      <c r="AB74" s="179"/>
+      <c r="AC74" s="179"/>
+      <c r="AD74" s="179"/>
+      <c r="AE74" s="179"/>
+      <c r="AF74" s="179"/>
+      <c r="AG74" s="214"/>
+      <c r="AH74" s="178" t="s">
         <v>66</v>
       </c>
-      <c r="AI74" s="187"/>
-      <c r="AJ74" s="187"/>
-      <c r="AK74" s="187"/>
-      <c r="AL74" s="187"/>
-      <c r="AM74" s="187"/>
+      <c r="AI74" s="179"/>
+      <c r="AJ74" s="179"/>
+      <c r="AK74" s="179"/>
+      <c r="AL74" s="179"/>
+      <c r="AM74" s="179"/>
       <c r="AN74" s="13"/>
       <c r="AO74" s="13"/>
       <c r="AP74" s="13"/>
@@ -8901,37 +8905,22 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="AH74:AM74"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="M3:P4"/>
-    <mergeCell ref="Q3:T4"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="AW3:AZ4"/>
-    <mergeCell ref="U2:AN2"/>
-    <mergeCell ref="AO2:BH2"/>
-    <mergeCell ref="Y3:AB4"/>
-    <mergeCell ref="AC3:AF4"/>
-    <mergeCell ref="AG3:AJ4"/>
-    <mergeCell ref="AK3:AN4"/>
-    <mergeCell ref="BE3:BH4"/>
-    <mergeCell ref="B71:D72"/>
-    <mergeCell ref="B69:D70"/>
-    <mergeCell ref="B67:D68"/>
-    <mergeCell ref="B65:D66"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B63:D64"/>
-    <mergeCell ref="B61:D62"/>
-    <mergeCell ref="B59:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="U3:X4"/>
+    <mergeCell ref="Q74:T74"/>
+    <mergeCell ref="BA3:BD4"/>
+    <mergeCell ref="AA74:AG74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="M74:O74"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="BI2:BL2"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
@@ -8948,22 +8937,37 @@
     <mergeCell ref="AO3:AR4"/>
     <mergeCell ref="AS3:AV4"/>
     <mergeCell ref="E2:T2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="U3:X4"/>
-    <mergeCell ref="Q74:T74"/>
-    <mergeCell ref="BA3:BD4"/>
-    <mergeCell ref="AA74:AG74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="M74:O74"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B71:D72"/>
+    <mergeCell ref="B69:D70"/>
+    <mergeCell ref="B67:D68"/>
+    <mergeCell ref="B65:D66"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B63:D64"/>
+    <mergeCell ref="B61:D62"/>
+    <mergeCell ref="B59:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="AW3:AZ4"/>
+    <mergeCell ref="U2:AN2"/>
+    <mergeCell ref="AO2:BH2"/>
+    <mergeCell ref="Y3:AB4"/>
+    <mergeCell ref="AC3:AF4"/>
+    <mergeCell ref="AG3:AJ4"/>
+    <mergeCell ref="AK3:AN4"/>
+    <mergeCell ref="BE3:BH4"/>
+    <mergeCell ref="AH74:AM74"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="Q3:T4"/>
+    <mergeCell ref="E3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
@@ -9271,21 +9275,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100501A2237DBCF164BB17DE35239A4E5F0" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d252ecba0bbb92ffcd60552382fd808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d5e11d0132dc5bb78ad0fb0e89938ac">
     <xsd:element name="properties">
@@ -9399,10 +9388,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9423,17 +9435,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemented Saving ILO-Query to JSON and updated docs
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F99636-2DAF-46CE-A176-9F20F5E54115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3431FF01-515C-4468-927C-FD2C34C9F764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1103,11 +1103,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1127,42 +1128,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1172,8 +1137,47 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1202,31 +1206,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -3594,7 +3594,7 @@
   <dimension ref="B1:BV74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE42" sqref="AE42:AF42"/>
+      <selection activeCell="AM44" sqref="AM44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,246 +3635,246 @@
   <sheetData>
     <row r="1" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="204" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="198" t="s">
+      <c r="C2" s="205"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="187" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="199"/>
-      <c r="L2" s="199"/>
-      <c r="M2" s="199"/>
-      <c r="N2" s="199"/>
-      <c r="O2" s="199"/>
-      <c r="P2" s="199"/>
-      <c r="Q2" s="199"/>
-      <c r="R2" s="199"/>
-      <c r="S2" s="199"/>
-      <c r="T2" s="200"/>
-      <c r="U2" s="198" t="s">
+      <c r="F2" s="188"/>
+      <c r="G2" s="188"/>
+      <c r="H2" s="188"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="188"/>
+      <c r="K2" s="188"/>
+      <c r="L2" s="188"/>
+      <c r="M2" s="188"/>
+      <c r="N2" s="188"/>
+      <c r="O2" s="188"/>
+      <c r="P2" s="188"/>
+      <c r="Q2" s="188"/>
+      <c r="R2" s="188"/>
+      <c r="S2" s="188"/>
+      <c r="T2" s="189"/>
+      <c r="U2" s="187" t="s">
         <v>61</v>
       </c>
-      <c r="V2" s="199"/>
-      <c r="W2" s="199"/>
-      <c r="X2" s="199"/>
-      <c r="Y2" s="199"/>
-      <c r="Z2" s="199"/>
-      <c r="AA2" s="199"/>
-      <c r="AB2" s="199"/>
-      <c r="AC2" s="199"/>
-      <c r="AD2" s="199"/>
-      <c r="AE2" s="199"/>
-      <c r="AF2" s="199"/>
-      <c r="AG2" s="199"/>
-      <c r="AH2" s="199"/>
-      <c r="AI2" s="199"/>
-      <c r="AJ2" s="199"/>
-      <c r="AK2" s="199"/>
-      <c r="AL2" s="199"/>
-      <c r="AM2" s="199"/>
-      <c r="AN2" s="200"/>
-      <c r="AO2" s="198" t="s">
+      <c r="V2" s="188"/>
+      <c r="W2" s="188"/>
+      <c r="X2" s="188"/>
+      <c r="Y2" s="188"/>
+      <c r="Z2" s="188"/>
+      <c r="AA2" s="188"/>
+      <c r="AB2" s="188"/>
+      <c r="AC2" s="188"/>
+      <c r="AD2" s="188"/>
+      <c r="AE2" s="188"/>
+      <c r="AF2" s="188"/>
+      <c r="AG2" s="188"/>
+      <c r="AH2" s="188"/>
+      <c r="AI2" s="188"/>
+      <c r="AJ2" s="188"/>
+      <c r="AK2" s="188"/>
+      <c r="AL2" s="188"/>
+      <c r="AM2" s="188"/>
+      <c r="AN2" s="189"/>
+      <c r="AO2" s="187" t="s">
         <v>62</v>
       </c>
-      <c r="AP2" s="199"/>
-      <c r="AQ2" s="199"/>
-      <c r="AR2" s="199"/>
-      <c r="AS2" s="199"/>
-      <c r="AT2" s="199"/>
-      <c r="AU2" s="199"/>
-      <c r="AV2" s="199"/>
-      <c r="AW2" s="199"/>
-      <c r="AX2" s="199"/>
-      <c r="AY2" s="199"/>
-      <c r="AZ2" s="199"/>
-      <c r="BA2" s="199"/>
-      <c r="BB2" s="199"/>
-      <c r="BC2" s="199"/>
-      <c r="BD2" s="199"/>
-      <c r="BE2" s="199"/>
-      <c r="BF2" s="199"/>
-      <c r="BG2" s="199"/>
-      <c r="BH2" s="200"/>
-      <c r="BI2" s="198" t="s">
+      <c r="AP2" s="188"/>
+      <c r="AQ2" s="188"/>
+      <c r="AR2" s="188"/>
+      <c r="AS2" s="188"/>
+      <c r="AT2" s="188"/>
+      <c r="AU2" s="188"/>
+      <c r="AV2" s="188"/>
+      <c r="AW2" s="188"/>
+      <c r="AX2" s="188"/>
+      <c r="AY2" s="188"/>
+      <c r="AZ2" s="188"/>
+      <c r="BA2" s="188"/>
+      <c r="BB2" s="188"/>
+      <c r="BC2" s="188"/>
+      <c r="BD2" s="188"/>
+      <c r="BE2" s="188"/>
+      <c r="BF2" s="188"/>
+      <c r="BG2" s="188"/>
+      <c r="BH2" s="189"/>
+      <c r="BI2" s="187" t="s">
         <v>63</v>
       </c>
-      <c r="BJ2" s="199"/>
-      <c r="BK2" s="199"/>
-      <c r="BL2" s="200"/>
+      <c r="BJ2" s="188"/>
+      <c r="BK2" s="188"/>
+      <c r="BL2" s="189"/>
     </row>
     <row r="3" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="205" t="s">
+      <c r="B3" s="207" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="206"/>
-      <c r="D3" s="209" t="s">
+      <c r="C3" s="208"/>
+      <c r="D3" s="211" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="180" t="s">
+      <c r="E3" s="181" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="182"/>
-      <c r="I3" s="180" t="s">
+      <c r="F3" s="182"/>
+      <c r="G3" s="182"/>
+      <c r="H3" s="183"/>
+      <c r="I3" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="181"/>
-      <c r="K3" s="181"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="180" t="s">
+      <c r="J3" s="182"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="183"/>
+      <c r="M3" s="181" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="181"/>
-      <c r="O3" s="181"/>
-      <c r="P3" s="182"/>
-      <c r="Q3" s="180" t="s">
+      <c r="N3" s="182"/>
+      <c r="O3" s="182"/>
+      <c r="P3" s="183"/>
+      <c r="Q3" s="181" t="s">
         <v>48</v>
       </c>
-      <c r="R3" s="181"/>
-      <c r="S3" s="181"/>
-      <c r="T3" s="182"/>
-      <c r="U3" s="180" t="s">
+      <c r="R3" s="182"/>
+      <c r="S3" s="182"/>
+      <c r="T3" s="183"/>
+      <c r="U3" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="V3" s="181"/>
-      <c r="W3" s="181"/>
-      <c r="X3" s="182"/>
-      <c r="Y3" s="180" t="s">
+      <c r="V3" s="182"/>
+      <c r="W3" s="182"/>
+      <c r="X3" s="183"/>
+      <c r="Y3" s="181" t="s">
         <v>50</v>
       </c>
-      <c r="Z3" s="181"/>
-      <c r="AA3" s="181"/>
-      <c r="AB3" s="182"/>
-      <c r="AC3" s="180" t="s">
+      <c r="Z3" s="182"/>
+      <c r="AA3" s="182"/>
+      <c r="AB3" s="183"/>
+      <c r="AC3" s="181" t="s">
         <v>51</v>
       </c>
-      <c r="AD3" s="181"/>
-      <c r="AE3" s="181"/>
-      <c r="AF3" s="182"/>
-      <c r="AG3" s="180" t="s">
+      <c r="AD3" s="182"/>
+      <c r="AE3" s="182"/>
+      <c r="AF3" s="183"/>
+      <c r="AG3" s="181" t="s">
         <v>52</v>
       </c>
-      <c r="AH3" s="181"/>
-      <c r="AI3" s="181"/>
-      <c r="AJ3" s="182"/>
-      <c r="AK3" s="180" t="s">
+      <c r="AH3" s="182"/>
+      <c r="AI3" s="182"/>
+      <c r="AJ3" s="183"/>
+      <c r="AK3" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="AL3" s="181"/>
-      <c r="AM3" s="181"/>
-      <c r="AN3" s="182"/>
-      <c r="AO3" s="180" t="s">
+      <c r="AL3" s="182"/>
+      <c r="AM3" s="182"/>
+      <c r="AN3" s="183"/>
+      <c r="AO3" s="181" t="s">
         <v>54</v>
       </c>
-      <c r="AP3" s="181"/>
-      <c r="AQ3" s="181"/>
-      <c r="AR3" s="182"/>
-      <c r="AS3" s="180" t="s">
+      <c r="AP3" s="182"/>
+      <c r="AQ3" s="182"/>
+      <c r="AR3" s="183"/>
+      <c r="AS3" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="AT3" s="181"/>
-      <c r="AU3" s="181"/>
-      <c r="AV3" s="182"/>
-      <c r="AW3" s="180" t="s">
+      <c r="AT3" s="182"/>
+      <c r="AU3" s="182"/>
+      <c r="AV3" s="183"/>
+      <c r="AW3" s="181" t="s">
         <v>56</v>
       </c>
-      <c r="AX3" s="181"/>
-      <c r="AY3" s="181"/>
-      <c r="AZ3" s="182"/>
-      <c r="BA3" s="180" t="s">
+      <c r="AX3" s="182"/>
+      <c r="AY3" s="182"/>
+      <c r="AZ3" s="183"/>
+      <c r="BA3" s="181" t="s">
         <v>57</v>
       </c>
-      <c r="BB3" s="181"/>
-      <c r="BC3" s="181"/>
-      <c r="BD3" s="182"/>
-      <c r="BE3" s="180" t="s">
+      <c r="BB3" s="182"/>
+      <c r="BC3" s="182"/>
+      <c r="BD3" s="183"/>
+      <c r="BE3" s="181" t="s">
         <v>58</v>
       </c>
-      <c r="BF3" s="181"/>
-      <c r="BG3" s="181"/>
-      <c r="BH3" s="182"/>
-      <c r="BI3" s="180" t="s">
+      <c r="BF3" s="182"/>
+      <c r="BG3" s="182"/>
+      <c r="BH3" s="183"/>
+      <c r="BI3" s="181" t="s">
         <v>59</v>
       </c>
-      <c r="BJ3" s="181"/>
-      <c r="BK3" s="181"/>
-      <c r="BL3" s="182"/>
+      <c r="BJ3" s="182"/>
+      <c r="BK3" s="182"/>
+      <c r="BL3" s="183"/>
     </row>
     <row r="4" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="207"/>
-      <c r="C4" s="208"/>
-      <c r="D4" s="210"/>
-      <c r="E4" s="183"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="185"/>
-      <c r="I4" s="183"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="185"/>
-      <c r="M4" s="183"/>
-      <c r="N4" s="184"/>
-      <c r="O4" s="184"/>
-      <c r="P4" s="185"/>
-      <c r="Q4" s="183"/>
-      <c r="R4" s="184"/>
-      <c r="S4" s="184"/>
-      <c r="T4" s="185"/>
-      <c r="U4" s="183"/>
-      <c r="V4" s="184"/>
-      <c r="W4" s="184"/>
-      <c r="X4" s="185"/>
-      <c r="Y4" s="183"/>
-      <c r="Z4" s="184"/>
-      <c r="AA4" s="184"/>
-      <c r="AB4" s="185"/>
-      <c r="AC4" s="183"/>
-      <c r="AD4" s="184"/>
-      <c r="AE4" s="184"/>
-      <c r="AF4" s="185"/>
-      <c r="AG4" s="183"/>
-      <c r="AH4" s="184"/>
-      <c r="AI4" s="184"/>
-      <c r="AJ4" s="185"/>
-      <c r="AK4" s="183"/>
-      <c r="AL4" s="184"/>
-      <c r="AM4" s="184"/>
-      <c r="AN4" s="185"/>
-      <c r="AO4" s="183"/>
-      <c r="AP4" s="184"/>
-      <c r="AQ4" s="184"/>
-      <c r="AR4" s="185"/>
-      <c r="AS4" s="183"/>
-      <c r="AT4" s="184"/>
-      <c r="AU4" s="184"/>
-      <c r="AV4" s="185"/>
-      <c r="AW4" s="183"/>
-      <c r="AX4" s="184"/>
-      <c r="AY4" s="184"/>
-      <c r="AZ4" s="185"/>
-      <c r="BA4" s="183"/>
-      <c r="BB4" s="184"/>
-      <c r="BC4" s="184"/>
-      <c r="BD4" s="185"/>
-      <c r="BE4" s="183"/>
-      <c r="BF4" s="184"/>
-      <c r="BG4" s="184"/>
-      <c r="BH4" s="185"/>
-      <c r="BI4" s="183"/>
-      <c r="BJ4" s="184"/>
-      <c r="BK4" s="184"/>
-      <c r="BL4" s="185"/>
+      <c r="B4" s="209"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="212"/>
+      <c r="E4" s="184"/>
+      <c r="F4" s="185"/>
+      <c r="G4" s="185"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="184"/>
+      <c r="J4" s="185"/>
+      <c r="K4" s="185"/>
+      <c r="L4" s="186"/>
+      <c r="M4" s="184"/>
+      <c r="N4" s="185"/>
+      <c r="O4" s="185"/>
+      <c r="P4" s="186"/>
+      <c r="Q4" s="184"/>
+      <c r="R4" s="185"/>
+      <c r="S4" s="185"/>
+      <c r="T4" s="186"/>
+      <c r="U4" s="184"/>
+      <c r="V4" s="185"/>
+      <c r="W4" s="185"/>
+      <c r="X4" s="186"/>
+      <c r="Y4" s="184"/>
+      <c r="Z4" s="185"/>
+      <c r="AA4" s="185"/>
+      <c r="AB4" s="186"/>
+      <c r="AC4" s="184"/>
+      <c r="AD4" s="185"/>
+      <c r="AE4" s="185"/>
+      <c r="AF4" s="186"/>
+      <c r="AG4" s="184"/>
+      <c r="AH4" s="185"/>
+      <c r="AI4" s="185"/>
+      <c r="AJ4" s="186"/>
+      <c r="AK4" s="184"/>
+      <c r="AL4" s="185"/>
+      <c r="AM4" s="185"/>
+      <c r="AN4" s="186"/>
+      <c r="AO4" s="184"/>
+      <c r="AP4" s="185"/>
+      <c r="AQ4" s="185"/>
+      <c r="AR4" s="186"/>
+      <c r="AS4" s="184"/>
+      <c r="AT4" s="185"/>
+      <c r="AU4" s="185"/>
+      <c r="AV4" s="186"/>
+      <c r="AW4" s="184"/>
+      <c r="AX4" s="185"/>
+      <c r="AY4" s="185"/>
+      <c r="AZ4" s="186"/>
+      <c r="BA4" s="184"/>
+      <c r="BB4" s="185"/>
+      <c r="BC4" s="185"/>
+      <c r="BD4" s="186"/>
+      <c r="BE4" s="184"/>
+      <c r="BF4" s="185"/>
+      <c r="BG4" s="185"/>
+      <c r="BH4" s="186"/>
+      <c r="BI4" s="184"/>
+      <c r="BJ4" s="185"/>
+      <c r="BK4" s="185"/>
+      <c r="BL4" s="186"/>
     </row>
     <row r="5" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B5" s="196" t="s">
+      <c r="B5" s="198" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="43" t="s">
@@ -3946,7 +3946,7 @@
       <c r="BL5" s="22"/>
     </row>
     <row r="6" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B6" s="201"/>
+      <c r="B6" s="202"/>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4016,7 +4016,7 @@
       <c r="BL6" s="25"/>
     </row>
     <row r="7" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B7" s="178" t="s">
+      <c r="B7" s="196" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4090,7 +4090,7 @@
       <c r="BL7" s="25"/>
     </row>
     <row r="8" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B8" s="179"/>
+      <c r="B8" s="197"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -4171,7 +4171,7 @@
       <c r="BV8" s="90"/>
     </row>
     <row r="9" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B9" s="178" t="s">
+      <c r="B9" s="196" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4245,7 +4245,7 @@
       <c r="BL9" s="25"/>
     </row>
     <row r="10" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B10" s="179"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="BV10" s="92"/>
     </row>
     <row r="11" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="196" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4399,7 +4399,7 @@
       <c r="BL11" s="25"/>
     </row>
     <row r="12" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="195"/>
+      <c r="B12" s="203"/>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
@@ -4471,7 +4471,7 @@
       <c r="BL12" s="31"/>
     </row>
     <row r="13" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B13" s="196" t="s">
+      <c r="B13" s="198" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="43" t="s">
@@ -4543,7 +4543,7 @@
       <c r="BL13" s="52"/>
     </row>
     <row r="14" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B14" s="201"/>
+      <c r="B14" s="202"/>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4613,7 +4613,7 @@
       <c r="BL14" s="25"/>
     </row>
     <row r="15" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B15" s="178" t="s">
+      <c r="B15" s="196" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -4689,7 +4689,7 @@
       <c r="BL15" s="25"/>
     </row>
     <row r="16" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B16" s="179"/>
+      <c r="B16" s="197"/>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
@@ -4763,7 +4763,7 @@
       <c r="BL16" s="25"/>
     </row>
     <row r="17" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B17" s="178" t="s">
+      <c r="B17" s="196" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -4839,7 +4839,7 @@
       <c r="BL17" s="25"/>
     </row>
     <row r="18" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B18" s="179"/>
+      <c r="B18" s="197"/>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="BL18" s="25"/>
     </row>
     <row r="19" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B19" s="178" t="s">
+      <c r="B19" s="196" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -4987,7 +4987,7 @@
       <c r="BL19" s="25"/>
     </row>
     <row r="20" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B20" s="179"/>
+      <c r="B20" s="197"/>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="BL20" s="25"/>
     </row>
     <row r="21" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B21" s="178" t="s">
+      <c r="B21" s="196" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5133,7 +5133,7 @@
       <c r="BL21" s="25"/>
     </row>
     <row r="22" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B22" s="179"/>
+      <c r="B22" s="197"/>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
@@ -5205,7 +5205,7 @@
       <c r="BL22" s="25"/>
     </row>
     <row r="23" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B23" s="178" t="s">
+      <c r="B23" s="196" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5279,7 +5279,7 @@
       <c r="BL23" s="25"/>
     </row>
     <row r="24" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="195"/>
+      <c r="B24" s="203"/>
       <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
@@ -5351,7 +5351,7 @@
       <c r="BL24" s="31"/>
     </row>
     <row r="25" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B25" s="196" t="s">
+      <c r="B25" s="198" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -5425,7 +5425,7 @@
       <c r="BL25" s="52"/>
     </row>
     <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="197"/>
+      <c r="B26" s="199"/>
       <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
@@ -5497,7 +5497,7 @@
       <c r="BL26" s="31"/>
     </row>
     <row r="27" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B27" s="196" t="s">
+      <c r="B27" s="198" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -5569,13 +5569,13 @@
       <c r="BL27" s="22"/>
     </row>
     <row r="28" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B28" s="201"/>
+      <c r="B28" s="202"/>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>25.25</v>
+        <v>29.25</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -5639,7 +5639,7 @@
       <c r="BL28" s="25"/>
     </row>
     <row r="29" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B29" s="178" t="s">
+      <c r="B29" s="196" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -5715,7 +5715,7 @@
       <c r="BL29" s="25"/>
     </row>
     <row r="30" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B30" s="179"/>
+      <c r="B30" s="197"/>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
@@ -5789,7 +5789,7 @@
       <c r="BL30" s="25"/>
     </row>
     <row r="31" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B31" s="178" t="s">
+      <c r="B31" s="196" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -5865,7 +5865,7 @@
       <c r="BL31" s="25"/>
     </row>
     <row r="32" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B32" s="179"/>
+      <c r="B32" s="197"/>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
@@ -5941,7 +5941,7 @@
       <c r="BL32" s="25"/>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B33" s="178" t="s">
+      <c r="B33" s="196" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -6017,7 +6017,7 @@
       <c r="BL33" s="25"/>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B34" s="179"/>
+      <c r="B34" s="197"/>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
@@ -6095,7 +6095,7 @@
       <c r="BL34" s="25"/>
     </row>
     <row r="35" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B35" s="178" t="s">
+      <c r="B35" s="196" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -6169,7 +6169,7 @@
       <c r="BL35" s="25"/>
     </row>
     <row r="36" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B36" s="179"/>
+      <c r="B36" s="197"/>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
@@ -6243,7 +6243,7 @@
       <c r="BL36" s="25"/>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B37" s="178" t="s">
+      <c r="B37" s="196" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -6317,7 +6317,7 @@
       <c r="BL37" s="25"/>
     </row>
     <row r="38" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B38" s="179"/>
+      <c r="B38" s="197"/>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="BL38" s="25"/>
     </row>
     <row r="39" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B39" s="178" t="s">
+      <c r="B39" s="196" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -6469,7 +6469,7 @@
       <c r="BL39" s="25"/>
     </row>
     <row r="40" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B40" s="179"/>
+      <c r="B40" s="197"/>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
@@ -6543,7 +6543,7 @@
       <c r="BL40" s="25"/>
     </row>
     <row r="41" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B41" s="178" t="s">
+      <c r="B41" s="196" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -6623,13 +6623,13 @@
       <c r="BL41" s="25"/>
     </row>
     <row r="42" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B42" s="179"/>
+      <c r="B42" s="197"/>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D42" s="88">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="E42" s="71"/>
       <c r="F42" s="69"/>
@@ -6673,8 +6673,12 @@
       <c r="AH42" s="24"/>
       <c r="AI42" s="24"/>
       <c r="AJ42" s="25"/>
-      <c r="AK42" s="71"/>
-      <c r="AL42" s="69"/>
+      <c r="AK42" s="71">
+        <v>2</v>
+      </c>
+      <c r="AL42" s="69">
+        <v>0.5</v>
+      </c>
       <c r="AM42" s="69"/>
       <c r="AN42" s="70"/>
       <c r="AO42" s="32"/>
@@ -6703,7 +6707,7 @@
       <c r="BL42" s="25"/>
     </row>
     <row r="43" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B43" s="178" t="s">
+      <c r="B43" s="196" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6783,13 +6787,13 @@
       <c r="BL43" s="25"/>
     </row>
     <row r="44" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B44" s="179"/>
+      <c r="B44" s="197"/>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="88">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E44" s="71"/>
       <c r="F44" s="69"/>
@@ -6824,7 +6828,9 @@
       <c r="AI44" s="24"/>
       <c r="AJ44" s="25"/>
       <c r="AK44" s="71"/>
-      <c r="AL44" s="69"/>
+      <c r="AL44" s="69">
+        <v>1.5</v>
+      </c>
       <c r="AM44" s="69"/>
       <c r="AN44" s="70"/>
       <c r="AO44" s="32"/>
@@ -6853,7 +6859,7 @@
       <c r="BL44" s="25"/>
     </row>
     <row r="45" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B45" s="178" t="s">
+      <c r="B45" s="196" t="s">
         <v>65</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -6929,7 +6935,7 @@
       <c r="BL45" s="25"/>
     </row>
     <row r="46" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B46" s="179"/>
+      <c r="B46" s="197"/>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
@@ -6999,7 +7005,7 @@
       <c r="BL46" s="25"/>
     </row>
     <row r="47" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B47" s="178" t="s">
+      <c r="B47" s="196" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -7079,7 +7085,7 @@
       <c r="BL47" s="25"/>
     </row>
     <row r="48" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="179"/>
+      <c r="B48" s="197"/>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
@@ -7149,7 +7155,7 @@
       <c r="BL48" s="25"/>
     </row>
     <row r="49" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B49" s="196" t="s">
+      <c r="B49" s="198" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="43" t="s">
@@ -7225,7 +7231,7 @@
       <c r="BL49" s="52"/>
     </row>
     <row r="50" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="197"/>
+      <c r="B50" s="199"/>
       <c r="C50" s="7" t="s">
         <v>3</v>
       </c>
@@ -7295,7 +7301,7 @@
       <c r="BL50" s="31"/>
     </row>
     <row r="51" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B51" s="196" t="s">
+      <c r="B51" s="198" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="43" t="s">
@@ -7371,7 +7377,7 @@
       <c r="BL51" s="52"/>
     </row>
     <row r="52" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="197"/>
+      <c r="B52" s="199"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -7441,7 +7447,7 @@
       <c r="BL52" s="31"/>
     </row>
     <row r="53" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B53" s="196" t="s">
+      <c r="B53" s="198" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="43" t="s">
@@ -7517,7 +7523,7 @@
       <c r="BL53" s="52"/>
     </row>
     <row r="54" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="197"/>
+      <c r="B54" s="199"/>
       <c r="C54" s="7" t="s">
         <v>3</v>
       </c>
@@ -7587,7 +7593,7 @@
       <c r="BL54" s="31"/>
     </row>
     <row r="55" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B55" s="196" t="s">
+      <c r="B55" s="198" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="43" t="s">
@@ -7685,7 +7691,7 @@
       <c r="BL55" s="110"/>
     </row>
     <row r="56" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="197"/>
+      <c r="B56" s="199"/>
       <c r="C56" s="7" t="s">
         <v>3</v>
       </c>
@@ -7724,7 +7730,7 @@
         <v>1.25</v>
       </c>
       <c r="Y56" s="107"/>
-      <c r="Z56" s="219">
+      <c r="Z56" s="178">
         <v>0.5</v>
       </c>
       <c r="AA56" s="107"/>
@@ -7769,7 +7775,7 @@
       <c r="BL56" s="31"/>
     </row>
     <row r="57" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B57" s="217" t="s">
+      <c r="B57" s="200" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="54"/>
@@ -7836,7 +7842,7 @@
       <c r="BL57" s="57"/>
     </row>
     <row r="58" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="218"/>
+      <c r="B58" s="201"/>
       <c r="C58" s="59"/>
       <c r="D58" s="60"/>
       <c r="E58" s="63"/>
@@ -7901,11 +7907,11 @@
       <c r="BL58" s="62"/>
     </row>
     <row r="59" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B59" s="211" t="s">
+      <c r="B59" s="190" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="212"/>
-      <c r="D59" s="213"/>
+      <c r="C59" s="191"/>
+      <c r="D59" s="192"/>
       <c r="E59" s="144"/>
       <c r="F59" s="145"/>
       <c r="G59" s="172"/>
@@ -7968,9 +7974,9 @@
       <c r="BL59" s="112"/>
     </row>
     <row r="60" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="214"/>
-      <c r="C60" s="215"/>
-      <c r="D60" s="216"/>
+      <c r="B60" s="193"/>
+      <c r="C60" s="194"/>
+      <c r="D60" s="195"/>
       <c r="E60" s="137"/>
       <c r="F60" s="142"/>
       <c r="G60" s="173"/>
@@ -8033,11 +8039,11 @@
       <c r="BL60" s="31"/>
     </row>
     <row r="61" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B61" s="211" t="s">
+      <c r="B61" s="190" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="212"/>
-      <c r="D61" s="213"/>
+      <c r="C61" s="191"/>
+      <c r="D61" s="192"/>
       <c r="E61" s="80"/>
       <c r="F61" s="145"/>
       <c r="G61" s="145"/>
@@ -8100,9 +8106,9 @@
       <c r="BL61" s="113"/>
     </row>
     <row r="62" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="214"/>
-      <c r="C62" s="215"/>
-      <c r="D62" s="216"/>
+      <c r="B62" s="193"/>
+      <c r="C62" s="194"/>
+      <c r="D62" s="195"/>
       <c r="E62" s="74"/>
       <c r="F62" s="142"/>
       <c r="G62" s="142"/>
@@ -8165,11 +8171,11 @@
       <c r="BL62" s="31"/>
     </row>
     <row r="63" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B63" s="211" t="s">
+      <c r="B63" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="212"/>
-      <c r="D63" s="213"/>
+      <c r="C63" s="191"/>
+      <c r="D63" s="192"/>
       <c r="E63" s="80"/>
       <c r="F63" s="78"/>
       <c r="G63" s="78"/>
@@ -8232,9 +8238,9 @@
       <c r="BL63" s="113"/>
     </row>
     <row r="64" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="214"/>
-      <c r="C64" s="215"/>
-      <c r="D64" s="216"/>
+      <c r="B64" s="193"/>
+      <c r="C64" s="194"/>
+      <c r="D64" s="195"/>
       <c r="E64" s="74"/>
       <c r="F64" s="73"/>
       <c r="G64" s="73"/>
@@ -8297,11 +8303,11 @@
       <c r="BL64" s="31"/>
     </row>
     <row r="65" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B65" s="211" t="s">
+      <c r="B65" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="212"/>
-      <c r="D65" s="213"/>
+      <c r="C65" s="191"/>
+      <c r="D65" s="192"/>
       <c r="E65" s="80"/>
       <c r="F65" s="78"/>
       <c r="G65" s="78"/>
@@ -8364,9 +8370,9 @@
       <c r="BL65" s="113"/>
     </row>
     <row r="66" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="214"/>
-      <c r="C66" s="215"/>
-      <c r="D66" s="216"/>
+      <c r="B66" s="193"/>
+      <c r="C66" s="194"/>
+      <c r="D66" s="195"/>
       <c r="E66" s="74"/>
       <c r="F66" s="73"/>
       <c r="G66" s="73"/>
@@ -8429,11 +8435,11 @@
       <c r="BL66" s="31"/>
     </row>
     <row r="67" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B67" s="211" t="s">
+      <c r="B67" s="190" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="212"/>
-      <c r="D67" s="213"/>
+      <c r="C67" s="191"/>
+      <c r="D67" s="192"/>
       <c r="E67" s="80"/>
       <c r="F67" s="78"/>
       <c r="G67" s="78"/>
@@ -8496,9 +8502,9 @@
       <c r="BL67" s="113"/>
     </row>
     <row r="68" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="214"/>
-      <c r="C68" s="215"/>
-      <c r="D68" s="216"/>
+      <c r="B68" s="193"/>
+      <c r="C68" s="194"/>
+      <c r="D68" s="195"/>
       <c r="E68" s="74"/>
       <c r="F68" s="73"/>
       <c r="G68" s="73"/>
@@ -8561,11 +8567,11 @@
       <c r="BL68" s="31"/>
     </row>
     <row r="69" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B69" s="211" t="s">
+      <c r="B69" s="190" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="212"/>
-      <c r="D69" s="213"/>
+      <c r="C69" s="191"/>
+      <c r="D69" s="192"/>
       <c r="E69" s="80"/>
       <c r="F69" s="78"/>
       <c r="G69" s="78"/>
@@ -8628,9 +8634,9 @@
       <c r="BL69" s="113"/>
     </row>
     <row r="70" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="214"/>
-      <c r="C70" s="215"/>
-      <c r="D70" s="216"/>
+      <c r="B70" s="193"/>
+      <c r="C70" s="194"/>
+      <c r="D70" s="195"/>
       <c r="E70" s="74"/>
       <c r="F70" s="73"/>
       <c r="G70" s="73"/>
@@ -8693,11 +8699,11 @@
       <c r="BL70" s="31"/>
     </row>
     <row r="71" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B71" s="211" t="s">
+      <c r="B71" s="190" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="212"/>
-      <c r="D71" s="213"/>
+      <c r="C71" s="191"/>
+      <c r="D71" s="192"/>
       <c r="E71" s="80"/>
       <c r="F71" s="78"/>
       <c r="G71" s="78"/>
@@ -8760,9 +8766,9 @@
       <c r="BL71" s="113"/>
     </row>
     <row r="72" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="214"/>
-      <c r="C72" s="215"/>
-      <c r="D72" s="216"/>
+      <c r="B72" s="193"/>
+      <c r="C72" s="194"/>
+      <c r="D72" s="195"/>
       <c r="E72" s="74"/>
       <c r="F72" s="73"/>
       <c r="G72" s="73"/>
@@ -8843,55 +8849,55 @@
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
-      <c r="E74" s="191" t="s">
+      <c r="E74" s="216" t="s">
         <v>2</v>
       </c>
-      <c r="F74" s="192"/>
-      <c r="G74" s="192"/>
+      <c r="F74" s="217"/>
+      <c r="G74" s="217"/>
       <c r="H74" s="64"/>
-      <c r="I74" s="191" t="s">
+      <c r="I74" s="216" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="192"/>
-      <c r="K74" s="192"/>
+      <c r="J74" s="217"/>
+      <c r="K74" s="217"/>
       <c r="L74" s="65"/>
-      <c r="M74" s="193" t="s">
+      <c r="M74" s="218" t="s">
         <v>14</v>
       </c>
-      <c r="N74" s="194"/>
-      <c r="O74" s="194"/>
+      <c r="N74" s="219"/>
+      <c r="O74" s="219"/>
       <c r="P74" s="66"/>
-      <c r="Q74" s="186" t="s">
+      <c r="Q74" s="213" t="s">
         <v>15</v>
       </c>
-      <c r="R74" s="187"/>
-      <c r="S74" s="187"/>
-      <c r="T74" s="187"/>
+      <c r="R74" s="214"/>
+      <c r="S74" s="214"/>
+      <c r="T74" s="214"/>
       <c r="U74" s="67"/>
       <c r="V74" s="135"/>
-      <c r="W74" s="187" t="s">
+      <c r="W74" s="214" t="s">
         <v>28</v>
       </c>
-      <c r="X74" s="187"/>
-      <c r="Y74" s="187"/>
+      <c r="X74" s="214"/>
+      <c r="Y74" s="214"/>
       <c r="Z74" s="68"/>
-      <c r="AA74" s="188" t="s">
+      <c r="AA74" s="179" t="s">
         <v>64</v>
       </c>
-      <c r="AB74" s="189"/>
-      <c r="AC74" s="189"/>
-      <c r="AD74" s="189"/>
-      <c r="AE74" s="189"/>
-      <c r="AF74" s="189"/>
-      <c r="AG74" s="190"/>
-      <c r="AH74" s="188" t="s">
+      <c r="AB74" s="180"/>
+      <c r="AC74" s="180"/>
+      <c r="AD74" s="180"/>
+      <c r="AE74" s="180"/>
+      <c r="AF74" s="180"/>
+      <c r="AG74" s="215"/>
+      <c r="AH74" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="AI74" s="189"/>
-      <c r="AJ74" s="189"/>
-      <c r="AK74" s="189"/>
-      <c r="AL74" s="189"/>
-      <c r="AM74" s="189"/>
+      <c r="AI74" s="180"/>
+      <c r="AJ74" s="180"/>
+      <c r="AK74" s="180"/>
+      <c r="AL74" s="180"/>
+      <c r="AM74" s="180"/>
       <c r="AN74" s="13"/>
       <c r="AO74" s="13"/>
       <c r="AP74" s="13"/>
@@ -8920,37 +8926,22 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="AH74:AM74"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="M3:P4"/>
-    <mergeCell ref="Q3:T4"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="AW3:AZ4"/>
-    <mergeCell ref="U2:AN2"/>
-    <mergeCell ref="AO2:BH2"/>
-    <mergeCell ref="Y3:AB4"/>
-    <mergeCell ref="AC3:AF4"/>
-    <mergeCell ref="AG3:AJ4"/>
-    <mergeCell ref="AK3:AN4"/>
-    <mergeCell ref="BE3:BH4"/>
-    <mergeCell ref="B71:D72"/>
-    <mergeCell ref="B69:D70"/>
-    <mergeCell ref="B67:D68"/>
-    <mergeCell ref="B65:D66"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B63:D64"/>
-    <mergeCell ref="B61:D62"/>
-    <mergeCell ref="B59:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="U3:X4"/>
+    <mergeCell ref="Q74:T74"/>
+    <mergeCell ref="BA3:BD4"/>
+    <mergeCell ref="AA74:AG74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="M74:O74"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="BI2:BL2"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
@@ -8967,22 +8958,37 @@
     <mergeCell ref="AO3:AR4"/>
     <mergeCell ref="AS3:AV4"/>
     <mergeCell ref="E2:T2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="U3:X4"/>
-    <mergeCell ref="Q74:T74"/>
-    <mergeCell ref="BA3:BD4"/>
-    <mergeCell ref="AA74:AG74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="M74:O74"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B71:D72"/>
+    <mergeCell ref="B69:D70"/>
+    <mergeCell ref="B67:D68"/>
+    <mergeCell ref="B65:D66"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B63:D64"/>
+    <mergeCell ref="B61:D62"/>
+    <mergeCell ref="B59:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="AW3:AZ4"/>
+    <mergeCell ref="U2:AN2"/>
+    <mergeCell ref="AO2:BH2"/>
+    <mergeCell ref="Y3:AB4"/>
+    <mergeCell ref="AC3:AF4"/>
+    <mergeCell ref="AG3:AJ4"/>
+    <mergeCell ref="AK3:AN4"/>
+    <mergeCell ref="BE3:BH4"/>
+    <mergeCell ref="AH74:AM74"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="Q3:T4"/>
+    <mergeCell ref="E3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
@@ -9290,21 +9296,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100501A2237DBCF164BB17DE35239A4E5F0" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d252ecba0bbb92ffcd60552382fd808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d5e11d0132dc5bb78ad0fb0e89938ac">
     <xsd:element name="properties">
@@ -9418,10 +9409,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9442,17 +9456,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemented Standard Saving in CSV and a lot of fixes and improvements along the way
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3431FF01-515C-4468-927C-FD2C34C9F764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201A763-D4DD-4E98-BCED-EE37F34133B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,9 +174,6 @@
     <t>Fehlerbehandlung</t>
   </si>
   <si>
-    <t>Dienstag (04.03.2025)</t>
-  </si>
-  <si>
     <t>Mittwoch (05.03.2025)</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>1 Arbeitstag = 8,3h</t>
+  </si>
+  <si>
+    <t>Dienstag   (04.03.2025)</t>
   </si>
 </sst>
 </file>
@@ -3593,8 +3593,8 @@
   </sheetPr>
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM44" sqref="AM44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BR21" sqref="BR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3615,7 +3615,7 @@
     <col min="21" max="23" width="4.28515625" customWidth="1"/>
     <col min="24" max="24" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="4.28515625" customWidth="1"/>
-    <col min="28" max="28" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="29" max="31" width="4.28515625" customWidth="1"/>
     <col min="32" max="32" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="35" width="4.28515625" customWidth="1"/>
@@ -3641,7 +3641,7 @@
       <c r="C2" s="205"/>
       <c r="D2" s="206"/>
       <c r="E2" s="187" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="188"/>
       <c r="G2" s="188"/>
@@ -3659,7 +3659,7 @@
       <c r="S2" s="188"/>
       <c r="T2" s="189"/>
       <c r="U2" s="187" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V2" s="188"/>
       <c r="W2" s="188"/>
@@ -3681,7 +3681,7 @@
       <c r="AM2" s="188"/>
       <c r="AN2" s="189"/>
       <c r="AO2" s="187" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AP2" s="188"/>
       <c r="AQ2" s="188"/>
@@ -3703,7 +3703,7 @@
       <c r="BG2" s="188"/>
       <c r="BH2" s="189"/>
       <c r="BI2" s="187" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BJ2" s="188"/>
       <c r="BK2" s="188"/>
@@ -3718,91 +3718,91 @@
         <v>17</v>
       </c>
       <c r="E3" s="181" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="F3" s="182"/>
       <c r="G3" s="182"/>
       <c r="H3" s="183"/>
       <c r="I3" s="181" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="182"/>
       <c r="K3" s="182"/>
       <c r="L3" s="183"/>
       <c r="M3" s="181" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N3" s="182"/>
       <c r="O3" s="182"/>
       <c r="P3" s="183"/>
       <c r="Q3" s="181" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R3" s="182"/>
       <c r="S3" s="182"/>
       <c r="T3" s="183"/>
       <c r="U3" s="181" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V3" s="182"/>
       <c r="W3" s="182"/>
       <c r="X3" s="183"/>
       <c r="Y3" s="181" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Z3" s="182"/>
       <c r="AA3" s="182"/>
       <c r="AB3" s="183"/>
       <c r="AC3" s="181" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AD3" s="182"/>
       <c r="AE3" s="182"/>
       <c r="AF3" s="183"/>
       <c r="AG3" s="181" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH3" s="182"/>
       <c r="AI3" s="182"/>
       <c r="AJ3" s="183"/>
       <c r="AK3" s="181" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AL3" s="182"/>
       <c r="AM3" s="182"/>
       <c r="AN3" s="183"/>
       <c r="AO3" s="181" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AP3" s="182"/>
       <c r="AQ3" s="182"/>
       <c r="AR3" s="183"/>
       <c r="AS3" s="181" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AT3" s="182"/>
       <c r="AU3" s="182"/>
       <c r="AV3" s="183"/>
       <c r="AW3" s="181" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AX3" s="182"/>
       <c r="AY3" s="182"/>
       <c r="AZ3" s="183"/>
       <c r="BA3" s="181" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BB3" s="182"/>
       <c r="BC3" s="182"/>
       <c r="BD3" s="183"/>
       <c r="BE3" s="181" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BF3" s="182"/>
       <c r="BG3" s="182"/>
       <c r="BH3" s="183"/>
       <c r="BI3" s="181" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BJ3" s="182"/>
       <c r="BK3" s="182"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>29.25</v>
+        <v>33.25</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -6673,10 +6673,10 @@
       <c r="AH42" s="24"/>
       <c r="AI42" s="24"/>
       <c r="AJ42" s="25"/>
-      <c r="AK42" s="71">
+      <c r="AK42" s="146">
         <v>2</v>
       </c>
-      <c r="AL42" s="69">
+      <c r="AL42" s="140">
         <v>0.5</v>
       </c>
       <c r="AM42" s="69"/>
@@ -6793,7 +6793,7 @@
       </c>
       <c r="D44" s="88">
         <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="E44" s="71"/>
       <c r="F44" s="69"/>
@@ -6828,11 +6828,15 @@
       <c r="AI44" s="24"/>
       <c r="AJ44" s="25"/>
       <c r="AK44" s="71"/>
-      <c r="AL44" s="69">
+      <c r="AL44" s="140">
         <v>1.5</v>
       </c>
-      <c r="AM44" s="69"/>
-      <c r="AN44" s="70"/>
+      <c r="AM44" s="140">
+        <v>2</v>
+      </c>
+      <c r="AN44" s="163">
+        <v>2</v>
+      </c>
       <c r="AO44" s="32"/>
       <c r="AP44" s="91"/>
       <c r="AQ44" s="16"/>
@@ -6860,7 +6864,7 @@
     </row>
     <row r="45" spans="2:64" x14ac:dyDescent="0.25">
       <c r="B45" s="196" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>2</v>
@@ -7161,7 +7165,7 @@
       <c r="C49" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D49" s="88">
+      <c r="D49" s="87">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -7697,7 +7701,7 @@
       </c>
       <c r="D56" s="88">
         <f>SUM(E56:BL56)</f>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
       <c r="E56" s="137">
         <v>1.5</v>
@@ -7734,7 +7738,9 @@
         <v>0.5</v>
       </c>
       <c r="AA56" s="107"/>
-      <c r="AB56" s="19"/>
+      <c r="AB56" s="164">
+        <v>0.25</v>
+      </c>
       <c r="AC56" s="29"/>
       <c r="AD56" s="30"/>
       <c r="AE56" s="107"/>
@@ -8882,7 +8888,7 @@
       <c r="Y74" s="214"/>
       <c r="Z74" s="68"/>
       <c r="AA74" s="179" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB74" s="180"/>
       <c r="AC74" s="180"/>
@@ -8891,7 +8897,7 @@
       <c r="AF74" s="180"/>
       <c r="AG74" s="215"/>
       <c r="AH74" s="179" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI74" s="180"/>
       <c r="AJ74" s="180"/>

</xml_diff>

<commit_message>
Working on Generation of Serial.csv, Updated docs
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B201A763-D4DD-4E98-BCED-EE37F34133B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B950BC8C-CDB0-4456-8AB1-6828CE8E30DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3593,8 +3593,8 @@
   </sheetPr>
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BR21" sqref="BR21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AN56" sqref="AN56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="D56" s="88">
         <f>SUM(E56:BL56)</f>
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
       <c r="E56" s="137">
         <v>1.5</v>
@@ -7754,7 +7754,9 @@
       <c r="AK56" s="53"/>
       <c r="AL56" s="35"/>
       <c r="AM56" s="18"/>
-      <c r="AN56" s="19"/>
+      <c r="AN56" s="164">
+        <v>0.25</v>
+      </c>
       <c r="AO56" s="109"/>
       <c r="AP56" s="131"/>
       <c r="AQ56" s="107"/>

</xml_diff>

<commit_message>
Small Fixes, Began implementing Help (Module help), reworked Get-Help to make it less function specific
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B950BC8C-CDB0-4456-8AB1-6828CE8E30DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9D5194-0BB3-4DE6-B55B-D6D18E867191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1104,11 +1104,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1128,6 +1128,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1137,47 +1173,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1206,26 +1203,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3594,7 +3594,7 @@
   <dimension ref="B1:BV74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AN56" sqref="AN56"/>
+      <selection activeCell="AQ46" sqref="AQ46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3635,86 +3635,86 @@
   <sheetData>
     <row r="1" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="203" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="205"/>
-      <c r="D2" s="206"/>
-      <c r="E2" s="187" t="s">
+      <c r="C2" s="204"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="199" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="188"/>
-      <c r="K2" s="188"/>
-      <c r="L2" s="188"/>
-      <c r="M2" s="188"/>
-      <c r="N2" s="188"/>
-      <c r="O2" s="188"/>
-      <c r="P2" s="188"/>
-      <c r="Q2" s="188"/>
-      <c r="R2" s="188"/>
-      <c r="S2" s="188"/>
-      <c r="T2" s="189"/>
-      <c r="U2" s="187" t="s">
+      <c r="F2" s="200"/>
+      <c r="G2" s="200"/>
+      <c r="H2" s="200"/>
+      <c r="I2" s="200"/>
+      <c r="J2" s="200"/>
+      <c r="K2" s="200"/>
+      <c r="L2" s="200"/>
+      <c r="M2" s="200"/>
+      <c r="N2" s="200"/>
+      <c r="O2" s="200"/>
+      <c r="P2" s="200"/>
+      <c r="Q2" s="200"/>
+      <c r="R2" s="200"/>
+      <c r="S2" s="200"/>
+      <c r="T2" s="201"/>
+      <c r="U2" s="199" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="188"/>
-      <c r="W2" s="188"/>
-      <c r="X2" s="188"/>
-      <c r="Y2" s="188"/>
-      <c r="Z2" s="188"/>
-      <c r="AA2" s="188"/>
-      <c r="AB2" s="188"/>
-      <c r="AC2" s="188"/>
-      <c r="AD2" s="188"/>
-      <c r="AE2" s="188"/>
-      <c r="AF2" s="188"/>
-      <c r="AG2" s="188"/>
-      <c r="AH2" s="188"/>
-      <c r="AI2" s="188"/>
-      <c r="AJ2" s="188"/>
-      <c r="AK2" s="188"/>
-      <c r="AL2" s="188"/>
-      <c r="AM2" s="188"/>
-      <c r="AN2" s="189"/>
-      <c r="AO2" s="187" t="s">
+      <c r="V2" s="200"/>
+      <c r="W2" s="200"/>
+      <c r="X2" s="200"/>
+      <c r="Y2" s="200"/>
+      <c r="Z2" s="200"/>
+      <c r="AA2" s="200"/>
+      <c r="AB2" s="200"/>
+      <c r="AC2" s="200"/>
+      <c r="AD2" s="200"/>
+      <c r="AE2" s="200"/>
+      <c r="AF2" s="200"/>
+      <c r="AG2" s="200"/>
+      <c r="AH2" s="200"/>
+      <c r="AI2" s="200"/>
+      <c r="AJ2" s="200"/>
+      <c r="AK2" s="200"/>
+      <c r="AL2" s="200"/>
+      <c r="AM2" s="200"/>
+      <c r="AN2" s="201"/>
+      <c r="AO2" s="199" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" s="188"/>
-      <c r="AQ2" s="188"/>
-      <c r="AR2" s="188"/>
-      <c r="AS2" s="188"/>
-      <c r="AT2" s="188"/>
-      <c r="AU2" s="188"/>
-      <c r="AV2" s="188"/>
-      <c r="AW2" s="188"/>
-      <c r="AX2" s="188"/>
-      <c r="AY2" s="188"/>
-      <c r="AZ2" s="188"/>
-      <c r="BA2" s="188"/>
-      <c r="BB2" s="188"/>
-      <c r="BC2" s="188"/>
-      <c r="BD2" s="188"/>
-      <c r="BE2" s="188"/>
-      <c r="BF2" s="188"/>
-      <c r="BG2" s="188"/>
-      <c r="BH2" s="189"/>
-      <c r="BI2" s="187" t="s">
+      <c r="AP2" s="200"/>
+      <c r="AQ2" s="200"/>
+      <c r="AR2" s="200"/>
+      <c r="AS2" s="200"/>
+      <c r="AT2" s="200"/>
+      <c r="AU2" s="200"/>
+      <c r="AV2" s="200"/>
+      <c r="AW2" s="200"/>
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="200"/>
+      <c r="AZ2" s="200"/>
+      <c r="BA2" s="200"/>
+      <c r="BB2" s="200"/>
+      <c r="BC2" s="200"/>
+      <c r="BD2" s="200"/>
+      <c r="BE2" s="200"/>
+      <c r="BF2" s="200"/>
+      <c r="BG2" s="200"/>
+      <c r="BH2" s="201"/>
+      <c r="BI2" s="199" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" s="188"/>
-      <c r="BK2" s="188"/>
-      <c r="BL2" s="189"/>
+      <c r="BJ2" s="200"/>
+      <c r="BK2" s="200"/>
+      <c r="BL2" s="201"/>
     </row>
     <row r="3" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="208"/>
-      <c r="D3" s="211" t="s">
+      <c r="C3" s="207"/>
+      <c r="D3" s="210" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="181" t="s">
@@ -3809,9 +3809,9 @@
       <c r="BL3" s="183"/>
     </row>
     <row r="4" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="209"/>
-      <c r="C4" s="210"/>
-      <c r="D4" s="212"/>
+      <c r="B4" s="208"/>
+      <c r="C4" s="209"/>
+      <c r="D4" s="211"/>
       <c r="E4" s="184"/>
       <c r="F4" s="185"/>
       <c r="G4" s="185"/>
@@ -3874,7 +3874,7 @@
       <c r="BL4" s="186"/>
     </row>
     <row r="5" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B5" s="198" t="s">
+      <c r="B5" s="197" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="43" t="s">
@@ -4016,7 +4016,7 @@
       <c r="BL6" s="25"/>
     </row>
     <row r="7" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="179" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4090,7 +4090,7 @@
       <c r="BL7" s="25"/>
     </row>
     <row r="8" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B8" s="197"/>
+      <c r="B8" s="180"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -4171,7 +4171,7 @@
       <c r="BV8" s="90"/>
     </row>
     <row r="9" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B9" s="196" t="s">
+      <c r="B9" s="179" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4245,7 +4245,7 @@
       <c r="BL9" s="25"/>
     </row>
     <row r="10" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B10" s="197"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4325,7 +4325,7 @@
       <c r="BV10" s="92"/>
     </row>
     <row r="11" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="179" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4399,7 +4399,7 @@
       <c r="BL11" s="25"/>
     </row>
     <row r="12" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="203"/>
+      <c r="B12" s="196"/>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
@@ -4471,7 +4471,7 @@
       <c r="BL12" s="31"/>
     </row>
     <row r="13" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B13" s="198" t="s">
+      <c r="B13" s="197" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="43" t="s">
@@ -4613,7 +4613,7 @@
       <c r="BL14" s="25"/>
     </row>
     <row r="15" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B15" s="196" t="s">
+      <c r="B15" s="179" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -4689,7 +4689,7 @@
       <c r="BL15" s="25"/>
     </row>
     <row r="16" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B16" s="197"/>
+      <c r="B16" s="180"/>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
@@ -4763,7 +4763,7 @@
       <c r="BL16" s="25"/>
     </row>
     <row r="17" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B17" s="196" t="s">
+      <c r="B17" s="179" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -4839,7 +4839,7 @@
       <c r="BL17" s="25"/>
     </row>
     <row r="18" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B18" s="197"/>
+      <c r="B18" s="180"/>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4913,7 +4913,7 @@
       <c r="BL18" s="25"/>
     </row>
     <row r="19" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B19" s="196" t="s">
+      <c r="B19" s="179" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -4987,7 +4987,7 @@
       <c r="BL19" s="25"/>
     </row>
     <row r="20" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B20" s="197"/>
+      <c r="B20" s="180"/>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="BL20" s="25"/>
     </row>
     <row r="21" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B21" s="196" t="s">
+      <c r="B21" s="179" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5133,7 +5133,7 @@
       <c r="BL21" s="25"/>
     </row>
     <row r="22" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B22" s="197"/>
+      <c r="B22" s="180"/>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
@@ -5205,7 +5205,7 @@
       <c r="BL22" s="25"/>
     </row>
     <row r="23" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B23" s="196" t="s">
+      <c r="B23" s="179" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5279,7 +5279,7 @@
       <c r="BL23" s="25"/>
     </row>
     <row r="24" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="203"/>
+      <c r="B24" s="196"/>
       <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
@@ -5351,7 +5351,7 @@
       <c r="BL24" s="31"/>
     </row>
     <row r="25" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B25" s="198" t="s">
+      <c r="B25" s="197" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -5425,7 +5425,7 @@
       <c r="BL25" s="52"/>
     </row>
     <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="199"/>
+      <c r="B26" s="198"/>
       <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
@@ -5497,7 +5497,7 @@
       <c r="BL26" s="31"/>
     </row>
     <row r="27" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B27" s="198" t="s">
+      <c r="B27" s="197" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>33.25</v>
+        <v>36.75</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -5639,7 +5639,7 @@
       <c r="BL28" s="25"/>
     </row>
     <row r="29" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B29" s="196" t="s">
+      <c r="B29" s="179" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -5715,7 +5715,7 @@
       <c r="BL29" s="25"/>
     </row>
     <row r="30" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B30" s="197"/>
+      <c r="B30" s="180"/>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
@@ -5789,7 +5789,7 @@
       <c r="BL30" s="25"/>
     </row>
     <row r="31" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B31" s="196" t="s">
+      <c r="B31" s="179" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -5865,7 +5865,7 @@
       <c r="BL31" s="25"/>
     </row>
     <row r="32" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B32" s="197"/>
+      <c r="B32" s="180"/>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
@@ -5941,7 +5941,7 @@
       <c r="BL32" s="25"/>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B33" s="196" t="s">
+      <c r="B33" s="179" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -6017,7 +6017,7 @@
       <c r="BL33" s="25"/>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B34" s="197"/>
+      <c r="B34" s="180"/>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
@@ -6095,7 +6095,7 @@
       <c r="BL34" s="25"/>
     </row>
     <row r="35" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B35" s="196" t="s">
+      <c r="B35" s="179" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -6169,7 +6169,7 @@
       <c r="BL35" s="25"/>
     </row>
     <row r="36" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B36" s="197"/>
+      <c r="B36" s="180"/>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
@@ -6243,7 +6243,7 @@
       <c r="BL36" s="25"/>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B37" s="196" t="s">
+      <c r="B37" s="179" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -6317,7 +6317,7 @@
       <c r="BL37" s="25"/>
     </row>
     <row r="38" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B38" s="197"/>
+      <c r="B38" s="180"/>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="BL38" s="25"/>
     </row>
     <row r="39" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B39" s="196" t="s">
+      <c r="B39" s="179" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -6469,7 +6469,7 @@
       <c r="BL39" s="25"/>
     </row>
     <row r="40" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B40" s="197"/>
+      <c r="B40" s="180"/>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
@@ -6543,7 +6543,7 @@
       <c r="BL40" s="25"/>
     </row>
     <row r="41" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B41" s="196" t="s">
+      <c r="B41" s="179" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -6623,7 +6623,7 @@
       <c r="BL41" s="25"/>
     </row>
     <row r="42" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B42" s="197"/>
+      <c r="B42" s="180"/>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="BL42" s="25"/>
     </row>
     <row r="43" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B43" s="196" t="s">
+      <c r="B43" s="179" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6787,13 +6787,13 @@
       <c r="BL43" s="25"/>
     </row>
     <row r="44" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B44" s="197"/>
+      <c r="B44" s="180"/>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="88">
         <f t="shared" si="2"/>
-        <v>5.5</v>
+        <v>9</v>
       </c>
       <c r="E44" s="71"/>
       <c r="F44" s="69"/>
@@ -6837,8 +6837,12 @@
       <c r="AN44" s="163">
         <v>2</v>
       </c>
-      <c r="AO44" s="32"/>
-      <c r="AP44" s="91"/>
+      <c r="AO44" s="32">
+        <v>2</v>
+      </c>
+      <c r="AP44" s="91">
+        <v>1.5</v>
+      </c>
       <c r="AQ44" s="16"/>
       <c r="AR44" s="17"/>
       <c r="AS44" s="71"/>
@@ -6863,7 +6867,7 @@
       <c r="BL44" s="25"/>
     </row>
     <row r="45" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B45" s="196" t="s">
+      <c r="B45" s="179" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -6939,13 +6943,13 @@
       <c r="BL45" s="25"/>
     </row>
     <row r="46" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B46" s="197"/>
+      <c r="B46" s="180"/>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="88">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E46" s="71"/>
       <c r="F46" s="69"/>
@@ -6985,8 +6989,12 @@
       <c r="AN46" s="70"/>
       <c r="AO46" s="32"/>
       <c r="AP46" s="91"/>
-      <c r="AQ46" s="16"/>
-      <c r="AR46" s="17"/>
+      <c r="AQ46" s="16">
+        <v>1</v>
+      </c>
+      <c r="AR46" s="17">
+        <v>3</v>
+      </c>
       <c r="AS46" s="71"/>
       <c r="AT46" s="69"/>
       <c r="AU46" s="69"/>
@@ -7009,7 +7017,7 @@
       <c r="BL46" s="25"/>
     </row>
     <row r="47" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B47" s="196" t="s">
+      <c r="B47" s="179" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -7089,7 +7097,7 @@
       <c r="BL47" s="25"/>
     </row>
     <row r="48" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="197"/>
+      <c r="B48" s="180"/>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
@@ -7159,7 +7167,7 @@
       <c r="BL48" s="25"/>
     </row>
     <row r="49" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B49" s="198" t="s">
+      <c r="B49" s="197" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="43" t="s">
@@ -7235,7 +7243,7 @@
       <c r="BL49" s="52"/>
     </row>
     <row r="50" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="199"/>
+      <c r="B50" s="198"/>
       <c r="C50" s="7" t="s">
         <v>3</v>
       </c>
@@ -7305,7 +7313,7 @@
       <c r="BL50" s="31"/>
     </row>
     <row r="51" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B51" s="198" t="s">
+      <c r="B51" s="197" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="43" t="s">
@@ -7381,7 +7389,7 @@
       <c r="BL51" s="52"/>
     </row>
     <row r="52" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="199"/>
+      <c r="B52" s="198"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -7451,7 +7459,7 @@
       <c r="BL52" s="31"/>
     </row>
     <row r="53" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B53" s="198" t="s">
+      <c r="B53" s="197" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="43" t="s">
@@ -7527,7 +7535,7 @@
       <c r="BL53" s="52"/>
     </row>
     <row r="54" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="199"/>
+      <c r="B54" s="198"/>
       <c r="C54" s="7" t="s">
         <v>3</v>
       </c>
@@ -7597,7 +7605,7 @@
       <c r="BL54" s="31"/>
     </row>
     <row r="55" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B55" s="198" t="s">
+      <c r="B55" s="197" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="43" t="s">
@@ -7695,13 +7703,13 @@
       <c r="BL55" s="110"/>
     </row>
     <row r="56" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="199"/>
+      <c r="B56" s="198"/>
       <c r="C56" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D56" s="88">
         <f>SUM(E56:BL56)</f>
-        <v>5.75</v>
+        <v>6.25</v>
       </c>
       <c r="E56" s="137">
         <v>1.5</v>
@@ -7758,7 +7766,9 @@
         <v>0.25</v>
       </c>
       <c r="AO56" s="109"/>
-      <c r="AP56" s="131"/>
+      <c r="AP56" s="131">
+        <v>0.5</v>
+      </c>
       <c r="AQ56" s="107"/>
       <c r="AR56" s="19"/>
       <c r="AS56" s="109"/>
@@ -7783,7 +7793,7 @@
       <c r="BL56" s="31"/>
     </row>
     <row r="57" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B57" s="200" t="s">
+      <c r="B57" s="218" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="54"/>
@@ -7850,7 +7860,7 @@
       <c r="BL57" s="57"/>
     </row>
     <row r="58" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="201"/>
+      <c r="B58" s="219"/>
       <c r="C58" s="59"/>
       <c r="D58" s="60"/>
       <c r="E58" s="63"/>
@@ -7915,11 +7925,11 @@
       <c r="BL58" s="62"/>
     </row>
     <row r="59" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B59" s="190" t="s">
+      <c r="B59" s="212" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="191"/>
-      <c r="D59" s="192"/>
+      <c r="C59" s="213"/>
+      <c r="D59" s="214"/>
       <c r="E59" s="144"/>
       <c r="F59" s="145"/>
       <c r="G59" s="172"/>
@@ -7982,9 +7992,9 @@
       <c r="BL59" s="112"/>
     </row>
     <row r="60" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="193"/>
-      <c r="C60" s="194"/>
-      <c r="D60" s="195"/>
+      <c r="B60" s="215"/>
+      <c r="C60" s="216"/>
+      <c r="D60" s="217"/>
       <c r="E60" s="137"/>
       <c r="F60" s="142"/>
       <c r="G60" s="173"/>
@@ -8047,11 +8057,11 @@
       <c r="BL60" s="31"/>
     </row>
     <row r="61" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B61" s="190" t="s">
+      <c r="B61" s="212" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="191"/>
-      <c r="D61" s="192"/>
+      <c r="C61" s="213"/>
+      <c r="D61" s="214"/>
       <c r="E61" s="80"/>
       <c r="F61" s="145"/>
       <c r="G61" s="145"/>
@@ -8114,9 +8124,9 @@
       <c r="BL61" s="113"/>
     </row>
     <row r="62" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="193"/>
-      <c r="C62" s="194"/>
-      <c r="D62" s="195"/>
+      <c r="B62" s="215"/>
+      <c r="C62" s="216"/>
+      <c r="D62" s="217"/>
       <c r="E62" s="74"/>
       <c r="F62" s="142"/>
       <c r="G62" s="142"/>
@@ -8179,11 +8189,11 @@
       <c r="BL62" s="31"/>
     </row>
     <row r="63" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B63" s="190" t="s">
+      <c r="B63" s="212" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="191"/>
-      <c r="D63" s="192"/>
+      <c r="C63" s="213"/>
+      <c r="D63" s="214"/>
       <c r="E63" s="80"/>
       <c r="F63" s="78"/>
       <c r="G63" s="78"/>
@@ -8246,9 +8256,9 @@
       <c r="BL63" s="113"/>
     </row>
     <row r="64" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="193"/>
-      <c r="C64" s="194"/>
-      <c r="D64" s="195"/>
+      <c r="B64" s="215"/>
+      <c r="C64" s="216"/>
+      <c r="D64" s="217"/>
       <c r="E64" s="74"/>
       <c r="F64" s="73"/>
       <c r="G64" s="73"/>
@@ -8311,11 +8321,11 @@
       <c r="BL64" s="31"/>
     </row>
     <row r="65" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B65" s="190" t="s">
+      <c r="B65" s="212" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="191"/>
-      <c r="D65" s="192"/>
+      <c r="C65" s="213"/>
+      <c r="D65" s="214"/>
       <c r="E65" s="80"/>
       <c r="F65" s="78"/>
       <c r="G65" s="78"/>
@@ -8378,9 +8388,9 @@
       <c r="BL65" s="113"/>
     </row>
     <row r="66" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="193"/>
-      <c r="C66" s="194"/>
-      <c r="D66" s="195"/>
+      <c r="B66" s="215"/>
+      <c r="C66" s="216"/>
+      <c r="D66" s="217"/>
       <c r="E66" s="74"/>
       <c r="F66" s="73"/>
       <c r="G66" s="73"/>
@@ -8443,11 +8453,11 @@
       <c r="BL66" s="31"/>
     </row>
     <row r="67" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B67" s="190" t="s">
+      <c r="B67" s="212" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="191"/>
-      <c r="D67" s="192"/>
+      <c r="C67" s="213"/>
+      <c r="D67" s="214"/>
       <c r="E67" s="80"/>
       <c r="F67" s="78"/>
       <c r="G67" s="78"/>
@@ -8510,9 +8520,9 @@
       <c r="BL67" s="113"/>
     </row>
     <row r="68" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="193"/>
-      <c r="C68" s="194"/>
-      <c r="D68" s="195"/>
+      <c r="B68" s="215"/>
+      <c r="C68" s="216"/>
+      <c r="D68" s="217"/>
       <c r="E68" s="74"/>
       <c r="F68" s="73"/>
       <c r="G68" s="73"/>
@@ -8575,11 +8585,11 @@
       <c r="BL68" s="31"/>
     </row>
     <row r="69" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B69" s="190" t="s">
+      <c r="B69" s="212" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="191"/>
-      <c r="D69" s="192"/>
+      <c r="C69" s="213"/>
+      <c r="D69" s="214"/>
       <c r="E69" s="80"/>
       <c r="F69" s="78"/>
       <c r="G69" s="78"/>
@@ -8642,9 +8652,9 @@
       <c r="BL69" s="113"/>
     </row>
     <row r="70" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="193"/>
-      <c r="C70" s="194"/>
-      <c r="D70" s="195"/>
+      <c r="B70" s="215"/>
+      <c r="C70" s="216"/>
+      <c r="D70" s="217"/>
       <c r="E70" s="74"/>
       <c r="F70" s="73"/>
       <c r="G70" s="73"/>
@@ -8707,11 +8717,11 @@
       <c r="BL70" s="31"/>
     </row>
     <row r="71" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B71" s="190" t="s">
+      <c r="B71" s="212" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="191"/>
-      <c r="D71" s="192"/>
+      <c r="C71" s="213"/>
+      <c r="D71" s="214"/>
       <c r="E71" s="80"/>
       <c r="F71" s="78"/>
       <c r="G71" s="78"/>
@@ -8774,9 +8784,9 @@
       <c r="BL71" s="113"/>
     </row>
     <row r="72" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="193"/>
-      <c r="C72" s="194"/>
-      <c r="D72" s="195"/>
+      <c r="B72" s="215"/>
+      <c r="C72" s="216"/>
+      <c r="D72" s="217"/>
       <c r="E72" s="74"/>
       <c r="F72" s="73"/>
       <c r="G72" s="73"/>
@@ -8857,55 +8867,55 @@
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
-      <c r="E74" s="216" t="s">
+      <c r="E74" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="F74" s="217"/>
-      <c r="G74" s="217"/>
+      <c r="F74" s="193"/>
+      <c r="G74" s="193"/>
       <c r="H74" s="64"/>
-      <c r="I74" s="216" t="s">
+      <c r="I74" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="217"/>
-      <c r="K74" s="217"/>
+      <c r="J74" s="193"/>
+      <c r="K74" s="193"/>
       <c r="L74" s="65"/>
-      <c r="M74" s="218" t="s">
+      <c r="M74" s="194" t="s">
         <v>14</v>
       </c>
-      <c r="N74" s="219"/>
-      <c r="O74" s="219"/>
+      <c r="N74" s="195"/>
+      <c r="O74" s="195"/>
       <c r="P74" s="66"/>
-      <c r="Q74" s="213" t="s">
+      <c r="Q74" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="R74" s="214"/>
-      <c r="S74" s="214"/>
-      <c r="T74" s="214"/>
+      <c r="R74" s="188"/>
+      <c r="S74" s="188"/>
+      <c r="T74" s="188"/>
       <c r="U74" s="67"/>
       <c r="V74" s="135"/>
-      <c r="W74" s="214" t="s">
+      <c r="W74" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="X74" s="214"/>
-      <c r="Y74" s="214"/>
+      <c r="X74" s="188"/>
+      <c r="Y74" s="188"/>
       <c r="Z74" s="68"/>
-      <c r="AA74" s="179" t="s">
+      <c r="AA74" s="189" t="s">
         <v>63</v>
       </c>
-      <c r="AB74" s="180"/>
-      <c r="AC74" s="180"/>
-      <c r="AD74" s="180"/>
-      <c r="AE74" s="180"/>
-      <c r="AF74" s="180"/>
-      <c r="AG74" s="215"/>
-      <c r="AH74" s="179" t="s">
+      <c r="AB74" s="190"/>
+      <c r="AC74" s="190"/>
+      <c r="AD74" s="190"/>
+      <c r="AE74" s="190"/>
+      <c r="AF74" s="190"/>
+      <c r="AG74" s="191"/>
+      <c r="AH74" s="189" t="s">
         <v>65</v>
       </c>
-      <c r="AI74" s="180"/>
-      <c r="AJ74" s="180"/>
-      <c r="AK74" s="180"/>
-      <c r="AL74" s="180"/>
-      <c r="AM74" s="180"/>
+      <c r="AI74" s="190"/>
+      <c r="AJ74" s="190"/>
+      <c r="AK74" s="190"/>
+      <c r="AL74" s="190"/>
+      <c r="AM74" s="190"/>
       <c r="AN74" s="13"/>
       <c r="AO74" s="13"/>
       <c r="AP74" s="13"/>
@@ -8934,6 +8944,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="AH74:AM74"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="Q3:T4"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="AW3:AZ4"/>
+    <mergeCell ref="U2:AN2"/>
+    <mergeCell ref="AO2:BH2"/>
+    <mergeCell ref="Y3:AB4"/>
+    <mergeCell ref="AC3:AF4"/>
+    <mergeCell ref="AG3:AJ4"/>
+    <mergeCell ref="AK3:AN4"/>
+    <mergeCell ref="BE3:BH4"/>
+    <mergeCell ref="B71:D72"/>
+    <mergeCell ref="B69:D70"/>
+    <mergeCell ref="B67:D68"/>
+    <mergeCell ref="B65:D66"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B63:D64"/>
+    <mergeCell ref="B61:D62"/>
+    <mergeCell ref="B59:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="BI2:BL2"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="BI3:BL4"/>
+    <mergeCell ref="AO3:AR4"/>
+    <mergeCell ref="AS3:AV4"/>
+    <mergeCell ref="E2:T2"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="U3:X4"/>
@@ -8950,53 +9007,6 @@
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B49:B50"/>
-    <mergeCell ref="BI2:BL2"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="BI3:BL4"/>
-    <mergeCell ref="AO3:AR4"/>
-    <mergeCell ref="AS3:AV4"/>
-    <mergeCell ref="E2:T2"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B71:D72"/>
-    <mergeCell ref="B69:D70"/>
-    <mergeCell ref="B67:D68"/>
-    <mergeCell ref="B65:D66"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B63:D64"/>
-    <mergeCell ref="B61:D62"/>
-    <mergeCell ref="B59:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="AW3:AZ4"/>
-    <mergeCell ref="U2:AN2"/>
-    <mergeCell ref="AO2:BH2"/>
-    <mergeCell ref="Y3:AB4"/>
-    <mergeCell ref="AC3:AF4"/>
-    <mergeCell ref="AG3:AJ4"/>
-    <mergeCell ref="AK3:AN4"/>
-    <mergeCell ref="BE3:BH4"/>
-    <mergeCell ref="AH74:AM74"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="M3:P4"/>
-    <mergeCell ref="Q3:T4"/>
-    <mergeCell ref="E3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
@@ -9304,6 +9314,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100501A2237DBCF164BB17DE35239A4E5F0" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d252ecba0bbb92ffcd60552382fd808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d5e11d0132dc5bb78ad0fb0e89938ac">
     <xsd:element name="properties">
@@ -9417,33 +9442,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9464,9 +9466,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
small improvements after second call with expert, added some errorhandling
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1ED87E-69E0-43CA-9BAE-43C3B774FFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6315F315-4826-4F62-B20E-BAF53E2A6E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -924,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1104,11 +1104,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1128,42 +1129,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1173,8 +1138,47 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1203,31 +1207,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -3594,8 +3595,8 @@
   </sheetPr>
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR46" sqref="AQ46:AR46"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AR43" sqref="AR43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,246 +3637,246 @@
   <sheetData>
     <row r="1" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="203" t="s">
+      <c r="B2" s="205" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="204"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="199" t="s">
+      <c r="C2" s="206"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="188" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="200"/>
-      <c r="G2" s="200"/>
-      <c r="H2" s="200"/>
-      <c r="I2" s="200"/>
-      <c r="J2" s="200"/>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
-      <c r="M2" s="200"/>
-      <c r="N2" s="200"/>
-      <c r="O2" s="200"/>
-      <c r="P2" s="200"/>
-      <c r="Q2" s="200"/>
-      <c r="R2" s="200"/>
-      <c r="S2" s="200"/>
-      <c r="T2" s="201"/>
-      <c r="U2" s="199" t="s">
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
+      <c r="L2" s="189"/>
+      <c r="M2" s="189"/>
+      <c r="N2" s="189"/>
+      <c r="O2" s="189"/>
+      <c r="P2" s="189"/>
+      <c r="Q2" s="189"/>
+      <c r="R2" s="189"/>
+      <c r="S2" s="189"/>
+      <c r="T2" s="190"/>
+      <c r="U2" s="188" t="s">
         <v>60</v>
       </c>
-      <c r="V2" s="200"/>
-      <c r="W2" s="200"/>
-      <c r="X2" s="200"/>
-      <c r="Y2" s="200"/>
-      <c r="Z2" s="200"/>
-      <c r="AA2" s="200"/>
-      <c r="AB2" s="200"/>
-      <c r="AC2" s="200"/>
-      <c r="AD2" s="200"/>
-      <c r="AE2" s="200"/>
-      <c r="AF2" s="200"/>
-      <c r="AG2" s="200"/>
-      <c r="AH2" s="200"/>
-      <c r="AI2" s="200"/>
-      <c r="AJ2" s="200"/>
-      <c r="AK2" s="200"/>
-      <c r="AL2" s="200"/>
-      <c r="AM2" s="200"/>
-      <c r="AN2" s="201"/>
-      <c r="AO2" s="199" t="s">
+      <c r="V2" s="189"/>
+      <c r="W2" s="189"/>
+      <c r="X2" s="189"/>
+      <c r="Y2" s="189"/>
+      <c r="Z2" s="189"/>
+      <c r="AA2" s="189"/>
+      <c r="AB2" s="189"/>
+      <c r="AC2" s="189"/>
+      <c r="AD2" s="189"/>
+      <c r="AE2" s="189"/>
+      <c r="AF2" s="189"/>
+      <c r="AG2" s="189"/>
+      <c r="AH2" s="189"/>
+      <c r="AI2" s="189"/>
+      <c r="AJ2" s="189"/>
+      <c r="AK2" s="189"/>
+      <c r="AL2" s="189"/>
+      <c r="AM2" s="189"/>
+      <c r="AN2" s="190"/>
+      <c r="AO2" s="188" t="s">
         <v>61</v>
       </c>
-      <c r="AP2" s="200"/>
-      <c r="AQ2" s="200"/>
-      <c r="AR2" s="200"/>
-      <c r="AS2" s="200"/>
-      <c r="AT2" s="200"/>
-      <c r="AU2" s="200"/>
-      <c r="AV2" s="200"/>
-      <c r="AW2" s="200"/>
-      <c r="AX2" s="200"/>
-      <c r="AY2" s="200"/>
-      <c r="AZ2" s="200"/>
-      <c r="BA2" s="200"/>
-      <c r="BB2" s="200"/>
-      <c r="BC2" s="200"/>
-      <c r="BD2" s="200"/>
-      <c r="BE2" s="200"/>
-      <c r="BF2" s="200"/>
-      <c r="BG2" s="200"/>
-      <c r="BH2" s="201"/>
-      <c r="BI2" s="199" t="s">
+      <c r="AP2" s="189"/>
+      <c r="AQ2" s="189"/>
+      <c r="AR2" s="189"/>
+      <c r="AS2" s="189"/>
+      <c r="AT2" s="189"/>
+      <c r="AU2" s="189"/>
+      <c r="AV2" s="189"/>
+      <c r="AW2" s="189"/>
+      <c r="AX2" s="189"/>
+      <c r="AY2" s="189"/>
+      <c r="AZ2" s="189"/>
+      <c r="BA2" s="189"/>
+      <c r="BB2" s="189"/>
+      <c r="BC2" s="189"/>
+      <c r="BD2" s="189"/>
+      <c r="BE2" s="189"/>
+      <c r="BF2" s="189"/>
+      <c r="BG2" s="189"/>
+      <c r="BH2" s="190"/>
+      <c r="BI2" s="188" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" s="200"/>
-      <c r="BK2" s="200"/>
-      <c r="BL2" s="201"/>
+      <c r="BJ2" s="189"/>
+      <c r="BK2" s="189"/>
+      <c r="BL2" s="190"/>
     </row>
     <row r="3" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="206" t="s">
+      <c r="B3" s="208" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="207"/>
-      <c r="D3" s="210" t="s">
+      <c r="C3" s="209"/>
+      <c r="D3" s="212" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="181" t="s">
+      <c r="E3" s="182" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="182"/>
-      <c r="G3" s="182"/>
-      <c r="H3" s="183"/>
-      <c r="I3" s="181" t="s">
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="182" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="182"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="183"/>
-      <c r="M3" s="181" t="s">
+      <c r="J3" s="183"/>
+      <c r="K3" s="183"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="182" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="182"/>
-      <c r="O3" s="182"/>
-      <c r="P3" s="183"/>
-      <c r="Q3" s="181" t="s">
+      <c r="N3" s="183"/>
+      <c r="O3" s="183"/>
+      <c r="P3" s="184"/>
+      <c r="Q3" s="182" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="182"/>
-      <c r="S3" s="182"/>
-      <c r="T3" s="183"/>
-      <c r="U3" s="181" t="s">
+      <c r="R3" s="183"/>
+      <c r="S3" s="183"/>
+      <c r="T3" s="184"/>
+      <c r="U3" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="V3" s="182"/>
-      <c r="W3" s="182"/>
-      <c r="X3" s="183"/>
-      <c r="Y3" s="181" t="s">
+      <c r="V3" s="183"/>
+      <c r="W3" s="183"/>
+      <c r="X3" s="184"/>
+      <c r="Y3" s="182" t="s">
         <v>49</v>
       </c>
-      <c r="Z3" s="182"/>
-      <c r="AA3" s="182"/>
-      <c r="AB3" s="183"/>
-      <c r="AC3" s="181" t="s">
+      <c r="Z3" s="183"/>
+      <c r="AA3" s="183"/>
+      <c r="AB3" s="184"/>
+      <c r="AC3" s="182" t="s">
         <v>50</v>
       </c>
-      <c r="AD3" s="182"/>
-      <c r="AE3" s="182"/>
-      <c r="AF3" s="183"/>
-      <c r="AG3" s="181" t="s">
+      <c r="AD3" s="183"/>
+      <c r="AE3" s="183"/>
+      <c r="AF3" s="184"/>
+      <c r="AG3" s="182" t="s">
         <v>51</v>
       </c>
-      <c r="AH3" s="182"/>
-      <c r="AI3" s="182"/>
-      <c r="AJ3" s="183"/>
-      <c r="AK3" s="181" t="s">
+      <c r="AH3" s="183"/>
+      <c r="AI3" s="183"/>
+      <c r="AJ3" s="184"/>
+      <c r="AK3" s="182" t="s">
         <v>52</v>
       </c>
-      <c r="AL3" s="182"/>
-      <c r="AM3" s="182"/>
-      <c r="AN3" s="183"/>
-      <c r="AO3" s="181" t="s">
+      <c r="AL3" s="183"/>
+      <c r="AM3" s="183"/>
+      <c r="AN3" s="184"/>
+      <c r="AO3" s="182" t="s">
         <v>53</v>
       </c>
-      <c r="AP3" s="182"/>
-      <c r="AQ3" s="182"/>
-      <c r="AR3" s="183"/>
-      <c r="AS3" s="181" t="s">
+      <c r="AP3" s="183"/>
+      <c r="AQ3" s="183"/>
+      <c r="AR3" s="184"/>
+      <c r="AS3" s="182" t="s">
         <v>54</v>
       </c>
-      <c r="AT3" s="182"/>
-      <c r="AU3" s="182"/>
-      <c r="AV3" s="183"/>
-      <c r="AW3" s="181" t="s">
+      <c r="AT3" s="183"/>
+      <c r="AU3" s="183"/>
+      <c r="AV3" s="184"/>
+      <c r="AW3" s="182" t="s">
         <v>55</v>
       </c>
-      <c r="AX3" s="182"/>
-      <c r="AY3" s="182"/>
-      <c r="AZ3" s="183"/>
-      <c r="BA3" s="181" t="s">
+      <c r="AX3" s="183"/>
+      <c r="AY3" s="183"/>
+      <c r="AZ3" s="184"/>
+      <c r="BA3" s="182" t="s">
         <v>56</v>
       </c>
-      <c r="BB3" s="182"/>
-      <c r="BC3" s="182"/>
-      <c r="BD3" s="183"/>
-      <c r="BE3" s="181" t="s">
+      <c r="BB3" s="183"/>
+      <c r="BC3" s="183"/>
+      <c r="BD3" s="184"/>
+      <c r="BE3" s="182" t="s">
         <v>57</v>
       </c>
-      <c r="BF3" s="182"/>
-      <c r="BG3" s="182"/>
-      <c r="BH3" s="183"/>
-      <c r="BI3" s="181" t="s">
+      <c r="BF3" s="183"/>
+      <c r="BG3" s="183"/>
+      <c r="BH3" s="184"/>
+      <c r="BI3" s="182" t="s">
         <v>58</v>
       </c>
-      <c r="BJ3" s="182"/>
-      <c r="BK3" s="182"/>
-      <c r="BL3" s="183"/>
+      <c r="BJ3" s="183"/>
+      <c r="BK3" s="183"/>
+      <c r="BL3" s="184"/>
     </row>
     <row r="4" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="208"/>
-      <c r="C4" s="209"/>
-      <c r="D4" s="211"/>
-      <c r="E4" s="184"/>
-      <c r="F4" s="185"/>
-      <c r="G4" s="185"/>
-      <c r="H4" s="186"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="185"/>
-      <c r="K4" s="185"/>
-      <c r="L4" s="186"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="185"/>
-      <c r="O4" s="185"/>
-      <c r="P4" s="186"/>
-      <c r="Q4" s="184"/>
-      <c r="R4" s="185"/>
-      <c r="S4" s="185"/>
-      <c r="T4" s="186"/>
-      <c r="U4" s="184"/>
-      <c r="V4" s="185"/>
-      <c r="W4" s="185"/>
-      <c r="X4" s="186"/>
-      <c r="Y4" s="184"/>
-      <c r="Z4" s="185"/>
-      <c r="AA4" s="185"/>
-      <c r="AB4" s="186"/>
-      <c r="AC4" s="184"/>
-      <c r="AD4" s="185"/>
-      <c r="AE4" s="185"/>
-      <c r="AF4" s="186"/>
-      <c r="AG4" s="184"/>
-      <c r="AH4" s="185"/>
-      <c r="AI4" s="185"/>
-      <c r="AJ4" s="186"/>
-      <c r="AK4" s="184"/>
-      <c r="AL4" s="185"/>
-      <c r="AM4" s="185"/>
-      <c r="AN4" s="186"/>
-      <c r="AO4" s="184"/>
-      <c r="AP4" s="185"/>
-      <c r="AQ4" s="185"/>
-      <c r="AR4" s="186"/>
-      <c r="AS4" s="184"/>
-      <c r="AT4" s="185"/>
-      <c r="AU4" s="185"/>
-      <c r="AV4" s="186"/>
-      <c r="AW4" s="184"/>
-      <c r="AX4" s="185"/>
-      <c r="AY4" s="185"/>
-      <c r="AZ4" s="186"/>
-      <c r="BA4" s="184"/>
-      <c r="BB4" s="185"/>
-      <c r="BC4" s="185"/>
-      <c r="BD4" s="186"/>
-      <c r="BE4" s="184"/>
-      <c r="BF4" s="185"/>
-      <c r="BG4" s="185"/>
-      <c r="BH4" s="186"/>
-      <c r="BI4" s="184"/>
-      <c r="BJ4" s="185"/>
-      <c r="BK4" s="185"/>
-      <c r="BL4" s="186"/>
+      <c r="B4" s="210"/>
+      <c r="C4" s="211"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="185"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="185"/>
+      <c r="J4" s="186"/>
+      <c r="K4" s="186"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="185"/>
+      <c r="N4" s="186"/>
+      <c r="O4" s="186"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="185"/>
+      <c r="R4" s="186"/>
+      <c r="S4" s="186"/>
+      <c r="T4" s="187"/>
+      <c r="U4" s="185"/>
+      <c r="V4" s="186"/>
+      <c r="W4" s="186"/>
+      <c r="X4" s="187"/>
+      <c r="Y4" s="185"/>
+      <c r="Z4" s="186"/>
+      <c r="AA4" s="186"/>
+      <c r="AB4" s="187"/>
+      <c r="AC4" s="185"/>
+      <c r="AD4" s="186"/>
+      <c r="AE4" s="186"/>
+      <c r="AF4" s="187"/>
+      <c r="AG4" s="185"/>
+      <c r="AH4" s="186"/>
+      <c r="AI4" s="186"/>
+      <c r="AJ4" s="187"/>
+      <c r="AK4" s="185"/>
+      <c r="AL4" s="186"/>
+      <c r="AM4" s="186"/>
+      <c r="AN4" s="187"/>
+      <c r="AO4" s="185"/>
+      <c r="AP4" s="186"/>
+      <c r="AQ4" s="186"/>
+      <c r="AR4" s="187"/>
+      <c r="AS4" s="185"/>
+      <c r="AT4" s="186"/>
+      <c r="AU4" s="186"/>
+      <c r="AV4" s="187"/>
+      <c r="AW4" s="185"/>
+      <c r="AX4" s="186"/>
+      <c r="AY4" s="186"/>
+      <c r="AZ4" s="187"/>
+      <c r="BA4" s="185"/>
+      <c r="BB4" s="186"/>
+      <c r="BC4" s="186"/>
+      <c r="BD4" s="187"/>
+      <c r="BE4" s="185"/>
+      <c r="BF4" s="186"/>
+      <c r="BG4" s="186"/>
+      <c r="BH4" s="187"/>
+      <c r="BI4" s="185"/>
+      <c r="BJ4" s="186"/>
+      <c r="BK4" s="186"/>
+      <c r="BL4" s="187"/>
     </row>
     <row r="5" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="199" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="43" t="s">
@@ -3947,7 +3948,7 @@
       <c r="BL5" s="22"/>
     </row>
     <row r="6" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B6" s="202"/>
+      <c r="B6" s="203"/>
       <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4017,7 +4018,7 @@
       <c r="BL6" s="25"/>
     </row>
     <row r="7" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B7" s="179" t="s">
+      <c r="B7" s="197" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -4091,7 +4092,7 @@
       <c r="BL7" s="25"/>
     </row>
     <row r="8" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B8" s="180"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
@@ -4172,7 +4173,7 @@
       <c r="BV8" s="90"/>
     </row>
     <row r="9" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B9" s="179" t="s">
+      <c r="B9" s="197" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -4246,7 +4247,7 @@
       <c r="BL9" s="25"/>
     </row>
     <row r="10" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B10" s="180"/>
+      <c r="B10" s="198"/>
       <c r="C10" s="1" t="s">
         <v>3</v>
       </c>
@@ -4326,7 +4327,7 @@
       <c r="BV10" s="92"/>
     </row>
     <row r="11" spans="2:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="179" t="s">
+      <c r="B11" s="197" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -4400,7 +4401,7 @@
       <c r="BL11" s="25"/>
     </row>
     <row r="12" spans="2:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="196"/>
+      <c r="B12" s="204"/>
       <c r="C12" s="7" t="s">
         <v>3</v>
       </c>
@@ -4472,7 +4473,7 @@
       <c r="BL12" s="31"/>
     </row>
     <row r="13" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B13" s="197" t="s">
+      <c r="B13" s="199" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="43" t="s">
@@ -4544,7 +4545,7 @@
       <c r="BL13" s="52"/>
     </row>
     <row r="14" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B14" s="202"/>
+      <c r="B14" s="203"/>
       <c r="C14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4614,7 +4615,7 @@
       <c r="BL14" s="25"/>
     </row>
     <row r="15" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B15" s="179" t="s">
+      <c r="B15" s="197" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -4690,7 +4691,7 @@
       <c r="BL15" s="25"/>
     </row>
     <row r="16" spans="2:74" x14ac:dyDescent="0.25">
-      <c r="B16" s="180"/>
+      <c r="B16" s="198"/>
       <c r="C16" s="1" t="s">
         <v>3</v>
       </c>
@@ -4764,7 +4765,7 @@
       <c r="BL16" s="25"/>
     </row>
     <row r="17" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B17" s="179" t="s">
+      <c r="B17" s="197" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -4840,7 +4841,7 @@
       <c r="BL17" s="25"/>
     </row>
     <row r="18" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B18" s="180"/>
+      <c r="B18" s="198"/>
       <c r="C18" s="1" t="s">
         <v>3</v>
       </c>
@@ -4914,7 +4915,7 @@
       <c r="BL18" s="25"/>
     </row>
     <row r="19" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B19" s="179" t="s">
+      <c r="B19" s="197" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -4988,7 +4989,7 @@
       <c r="BL19" s="25"/>
     </row>
     <row r="20" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B20" s="180"/>
+      <c r="B20" s="198"/>
       <c r="C20" s="1" t="s">
         <v>3</v>
       </c>
@@ -5060,7 +5061,7 @@
       <c r="BL20" s="25"/>
     </row>
     <row r="21" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B21" s="179" t="s">
+      <c r="B21" s="197" t="s">
         <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -5134,7 +5135,7 @@
       <c r="BL21" s="25"/>
     </row>
     <row r="22" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B22" s="180"/>
+      <c r="B22" s="198"/>
       <c r="C22" s="1" t="s">
         <v>3</v>
       </c>
@@ -5206,7 +5207,7 @@
       <c r="BL22" s="25"/>
     </row>
     <row r="23" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B23" s="179" t="s">
+      <c r="B23" s="197" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -5280,7 +5281,7 @@
       <c r="BL23" s="25"/>
     </row>
     <row r="24" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="196"/>
+      <c r="B24" s="204"/>
       <c r="C24" s="7" t="s">
         <v>3</v>
       </c>
@@ -5352,7 +5353,7 @@
       <c r="BL24" s="31"/>
     </row>
     <row r="25" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B25" s="197" t="s">
+      <c r="B25" s="199" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="43" t="s">
@@ -5426,7 +5427,7 @@
       <c r="BL25" s="52"/>
     </row>
     <row r="26" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="198"/>
+      <c r="B26" s="200"/>
       <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
@@ -5498,7 +5499,7 @@
       <c r="BL26" s="31"/>
     </row>
     <row r="27" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B27" s="197" t="s">
+      <c r="B27" s="199" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="43" t="s">
@@ -5570,13 +5571,13 @@
       <c r="BL27" s="22"/>
     </row>
     <row r="28" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B28" s="202"/>
+      <c r="B28" s="203"/>
       <c r="C28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>36.75</v>
+        <v>38.75</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -5640,7 +5641,7 @@
       <c r="BL28" s="25"/>
     </row>
     <row r="29" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B29" s="179" t="s">
+      <c r="B29" s="197" t="s">
         <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -5716,7 +5717,7 @@
       <c r="BL29" s="25"/>
     </row>
     <row r="30" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B30" s="180"/>
+      <c r="B30" s="198"/>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
@@ -5790,7 +5791,7 @@
       <c r="BL30" s="25"/>
     </row>
     <row r="31" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B31" s="179" t="s">
+      <c r="B31" s="197" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -5866,7 +5867,7 @@
       <c r="BL31" s="25"/>
     </row>
     <row r="32" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B32" s="180"/>
+      <c r="B32" s="198"/>
       <c r="C32" s="1" t="s">
         <v>3</v>
       </c>
@@ -5942,7 +5943,7 @@
       <c r="BL32" s="25"/>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B33" s="179" t="s">
+      <c r="B33" s="197" t="s">
         <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -6018,7 +6019,7 @@
       <c r="BL33" s="25"/>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B34" s="180"/>
+      <c r="B34" s="198"/>
       <c r="C34" s="1" t="s">
         <v>3</v>
       </c>
@@ -6096,7 +6097,7 @@
       <c r="BL34" s="25"/>
     </row>
     <row r="35" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B35" s="179" t="s">
+      <c r="B35" s="197" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -6170,7 +6171,7 @@
       <c r="BL35" s="25"/>
     </row>
     <row r="36" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B36" s="180"/>
+      <c r="B36" s="198"/>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
@@ -6244,7 +6245,7 @@
       <c r="BL36" s="25"/>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="197" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -6318,7 +6319,7 @@
       <c r="BL37" s="25"/>
     </row>
     <row r="38" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B38" s="180"/>
+      <c r="B38" s="198"/>
       <c r="C38" s="1" t="s">
         <v>3</v>
       </c>
@@ -6390,7 +6391,7 @@
       <c r="BL38" s="25"/>
     </row>
     <row r="39" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B39" s="179" t="s">
+      <c r="B39" s="197" t="s">
         <v>40</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -6470,7 +6471,7 @@
       <c r="BL39" s="25"/>
     </row>
     <row r="40" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B40" s="180"/>
+      <c r="B40" s="198"/>
       <c r="C40" s="1" t="s">
         <v>3</v>
       </c>
@@ -6544,7 +6545,7 @@
       <c r="BL40" s="25"/>
     </row>
     <row r="41" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B41" s="179" t="s">
+      <c r="B41" s="197" t="s">
         <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -6624,7 +6625,7 @@
       <c r="BL41" s="25"/>
     </row>
     <row r="42" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B42" s="180"/>
+      <c r="B42" s="198"/>
       <c r="C42" s="1" t="s">
         <v>3</v>
       </c>
@@ -6708,7 +6709,7 @@
       <c r="BL42" s="25"/>
     </row>
     <row r="43" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B43" s="179" t="s">
+      <c r="B43" s="197" t="s">
         <v>43</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -6788,7 +6789,7 @@
       <c r="BL43" s="25"/>
     </row>
     <row r="44" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B44" s="180"/>
+      <c r="B44" s="198"/>
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
@@ -6868,7 +6869,7 @@
       <c r="BL44" s="25"/>
     </row>
     <row r="45" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B45" s="179" t="s">
+      <c r="B45" s="197" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -6944,7 +6945,7 @@
       <c r="BL45" s="25"/>
     </row>
     <row r="46" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B46" s="180"/>
+      <c r="B46" s="198"/>
       <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
@@ -7018,7 +7019,7 @@
       <c r="BL46" s="25"/>
     </row>
     <row r="47" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B47" s="179" t="s">
+      <c r="B47" s="197" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -7098,13 +7099,13 @@
       <c r="BL47" s="25"/>
     </row>
     <row r="48" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="180"/>
+      <c r="B48" s="198"/>
       <c r="C48" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D48" s="88">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E48" s="71"/>
       <c r="F48" s="69"/>
@@ -7146,7 +7147,9 @@
       <c r="AP48" s="91"/>
       <c r="AQ48" s="16"/>
       <c r="AR48" s="17"/>
-      <c r="AS48" s="71"/>
+      <c r="AS48" s="146">
+        <v>2</v>
+      </c>
       <c r="AT48" s="69"/>
       <c r="AU48" s="69"/>
       <c r="AV48" s="70"/>
@@ -7168,7 +7171,7 @@
       <c r="BL48" s="25"/>
     </row>
     <row r="49" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B49" s="197" t="s">
+      <c r="B49" s="199" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="43" t="s">
@@ -7244,7 +7247,7 @@
       <c r="BL49" s="52"/>
     </row>
     <row r="50" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="198"/>
+      <c r="B50" s="200"/>
       <c r="C50" s="7" t="s">
         <v>3</v>
       </c>
@@ -7314,7 +7317,7 @@
       <c r="BL50" s="31"/>
     </row>
     <row r="51" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B51" s="197" t="s">
+      <c r="B51" s="199" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="43" t="s">
@@ -7390,7 +7393,7 @@
       <c r="BL51" s="52"/>
     </row>
     <row r="52" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="198"/>
+      <c r="B52" s="200"/>
       <c r="C52" s="7" t="s">
         <v>3</v>
       </c>
@@ -7460,7 +7463,7 @@
       <c r="BL52" s="31"/>
     </row>
     <row r="53" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B53" s="197" t="s">
+      <c r="B53" s="199" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="43" t="s">
@@ -7536,7 +7539,7 @@
       <c r="BL53" s="52"/>
     </row>
     <row r="54" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="198"/>
+      <c r="B54" s="200"/>
       <c r="C54" s="7" t="s">
         <v>3</v>
       </c>
@@ -7606,7 +7609,7 @@
       <c r="BL54" s="31"/>
     </row>
     <row r="55" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B55" s="197" t="s">
+      <c r="B55" s="199" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="43" t="s">
@@ -7704,7 +7707,7 @@
       <c r="BL55" s="110"/>
     </row>
     <row r="56" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="198"/>
+      <c r="B56" s="200"/>
       <c r="C56" s="7" t="s">
         <v>3</v>
       </c>
@@ -7767,7 +7770,7 @@
         <v>0.25</v>
       </c>
       <c r="AO56" s="109"/>
-      <c r="AP56" s="220">
+      <c r="AP56" s="179">
         <v>0.5</v>
       </c>
       <c r="AQ56" s="107"/>
@@ -7796,7 +7799,7 @@
       <c r="BL56" s="31"/>
     </row>
     <row r="57" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B57" s="218" t="s">
+      <c r="B57" s="201" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="54"/>
@@ -7863,7 +7866,7 @@
       <c r="BL57" s="57"/>
     </row>
     <row r="58" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="219"/>
+      <c r="B58" s="202"/>
       <c r="C58" s="59"/>
       <c r="D58" s="60"/>
       <c r="E58" s="63"/>
@@ -7928,11 +7931,11 @@
       <c r="BL58" s="62"/>
     </row>
     <row r="59" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B59" s="212" t="s">
+      <c r="B59" s="191" t="s">
         <v>1</v>
       </c>
-      <c r="C59" s="213"/>
-      <c r="D59" s="214"/>
+      <c r="C59" s="192"/>
+      <c r="D59" s="193"/>
       <c r="E59" s="144"/>
       <c r="F59" s="145"/>
       <c r="G59" s="172"/>
@@ -7995,9 +7998,9 @@
       <c r="BL59" s="112"/>
     </row>
     <row r="60" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="215"/>
-      <c r="C60" s="216"/>
-      <c r="D60" s="217"/>
+      <c r="B60" s="194"/>
+      <c r="C60" s="195"/>
+      <c r="D60" s="196"/>
       <c r="E60" s="137"/>
       <c r="F60" s="142"/>
       <c r="G60" s="173"/>
@@ -8060,11 +8063,11 @@
       <c r="BL60" s="31"/>
     </row>
     <row r="61" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B61" s="212" t="s">
+      <c r="B61" s="191" t="s">
         <v>4</v>
       </c>
-      <c r="C61" s="213"/>
-      <c r="D61" s="214"/>
+      <c r="C61" s="192"/>
+      <c r="D61" s="193"/>
       <c r="E61" s="80"/>
       <c r="F61" s="145"/>
       <c r="G61" s="145"/>
@@ -8127,9 +8130,9 @@
       <c r="BL61" s="113"/>
     </row>
     <row r="62" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="215"/>
-      <c r="C62" s="216"/>
-      <c r="D62" s="217"/>
+      <c r="B62" s="194"/>
+      <c r="C62" s="195"/>
+      <c r="D62" s="196"/>
       <c r="E62" s="74"/>
       <c r="F62" s="142"/>
       <c r="G62" s="142"/>
@@ -8192,11 +8195,11 @@
       <c r="BL62" s="31"/>
     </row>
     <row r="63" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B63" s="212" t="s">
+      <c r="B63" s="191" t="s">
         <v>5</v>
       </c>
-      <c r="C63" s="213"/>
-      <c r="D63" s="214"/>
+      <c r="C63" s="192"/>
+      <c r="D63" s="193"/>
       <c r="E63" s="80"/>
       <c r="F63" s="78"/>
       <c r="G63" s="78"/>
@@ -8259,9 +8262,9 @@
       <c r="BL63" s="113"/>
     </row>
     <row r="64" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="215"/>
-      <c r="C64" s="216"/>
-      <c r="D64" s="217"/>
+      <c r="B64" s="194"/>
+      <c r="C64" s="195"/>
+      <c r="D64" s="196"/>
       <c r="E64" s="74"/>
       <c r="F64" s="73"/>
       <c r="G64" s="73"/>
@@ -8324,11 +8327,11 @@
       <c r="BL64" s="31"/>
     </row>
     <row r="65" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B65" s="212" t="s">
+      <c r="B65" s="191" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="213"/>
-      <c r="D65" s="214"/>
+      <c r="C65" s="192"/>
+      <c r="D65" s="193"/>
       <c r="E65" s="80"/>
       <c r="F65" s="78"/>
       <c r="G65" s="78"/>
@@ -8391,9 +8394,9 @@
       <c r="BL65" s="113"/>
     </row>
     <row r="66" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="215"/>
-      <c r="C66" s="216"/>
-      <c r="D66" s="217"/>
+      <c r="B66" s="194"/>
+      <c r="C66" s="195"/>
+      <c r="D66" s="196"/>
       <c r="E66" s="74"/>
       <c r="F66" s="73"/>
       <c r="G66" s="73"/>
@@ -8412,29 +8415,29 @@
       <c r="T66" s="164"/>
       <c r="U66" s="137"/>
       <c r="V66" s="177"/>
-      <c r="W66" s="18"/>
-      <c r="X66" s="19"/>
-      <c r="Y66" s="35"/>
-      <c r="Z66" s="18"/>
-      <c r="AA66" s="18"/>
-      <c r="AB66" s="36"/>
+      <c r="W66" s="142"/>
+      <c r="X66" s="164"/>
+      <c r="Y66" s="177"/>
+      <c r="Z66" s="142"/>
+      <c r="AA66" s="142"/>
+      <c r="AB66" s="221"/>
       <c r="AC66" s="29"/>
       <c r="AD66" s="30"/>
-      <c r="AE66" s="18"/>
-      <c r="AF66" s="19"/>
+      <c r="AE66" s="142"/>
+      <c r="AF66" s="164"/>
       <c r="AG66" s="29"/>
       <c r="AH66" s="30"/>
       <c r="AI66" s="30"/>
       <c r="AJ66" s="31"/>
-      <c r="AK66" s="53"/>
-      <c r="AL66" s="35"/>
-      <c r="AM66" s="18"/>
-      <c r="AN66" s="19"/>
-      <c r="AO66" s="53"/>
-      <c r="AP66" s="35"/>
-      <c r="AQ66" s="18"/>
-      <c r="AR66" s="19"/>
-      <c r="AS66" s="53"/>
+      <c r="AK66" s="137"/>
+      <c r="AL66" s="177"/>
+      <c r="AM66" s="142"/>
+      <c r="AN66" s="164"/>
+      <c r="AO66" s="137"/>
+      <c r="AP66" s="177"/>
+      <c r="AQ66" s="142"/>
+      <c r="AR66" s="164"/>
+      <c r="AS66" s="137"/>
       <c r="AT66" s="18"/>
       <c r="AU66" s="18"/>
       <c r="AV66" s="19"/>
@@ -8456,11 +8459,11 @@
       <c r="BL66" s="31"/>
     </row>
     <row r="67" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B67" s="212" t="s">
+      <c r="B67" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="C67" s="213"/>
-      <c r="D67" s="214"/>
+      <c r="C67" s="192"/>
+      <c r="D67" s="193"/>
       <c r="E67" s="80"/>
       <c r="F67" s="78"/>
       <c r="G67" s="78"/>
@@ -8523,9 +8526,9 @@
       <c r="BL67" s="113"/>
     </row>
     <row r="68" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="215"/>
-      <c r="C68" s="216"/>
-      <c r="D68" s="217"/>
+      <c r="B68" s="194"/>
+      <c r="C68" s="195"/>
+      <c r="D68" s="196"/>
       <c r="E68" s="74"/>
       <c r="F68" s="73"/>
       <c r="G68" s="73"/>
@@ -8588,11 +8591,11 @@
       <c r="BL68" s="31"/>
     </row>
     <row r="69" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B69" s="212" t="s">
+      <c r="B69" s="191" t="s">
         <v>8</v>
       </c>
-      <c r="C69" s="213"/>
-      <c r="D69" s="214"/>
+      <c r="C69" s="192"/>
+      <c r="D69" s="193"/>
       <c r="E69" s="80"/>
       <c r="F69" s="78"/>
       <c r="G69" s="78"/>
@@ -8655,9 +8658,9 @@
       <c r="BL69" s="113"/>
     </row>
     <row r="70" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="215"/>
-      <c r="C70" s="216"/>
-      <c r="D70" s="217"/>
+      <c r="B70" s="194"/>
+      <c r="C70" s="195"/>
+      <c r="D70" s="196"/>
       <c r="E70" s="74"/>
       <c r="F70" s="73"/>
       <c r="G70" s="73"/>
@@ -8720,11 +8723,11 @@
       <c r="BL70" s="31"/>
     </row>
     <row r="71" spans="2:64" x14ac:dyDescent="0.25">
-      <c r="B71" s="212" t="s">
+      <c r="B71" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="C71" s="213"/>
-      <c r="D71" s="214"/>
+      <c r="C71" s="192"/>
+      <c r="D71" s="193"/>
       <c r="E71" s="80"/>
       <c r="F71" s="78"/>
       <c r="G71" s="78"/>
@@ -8787,9 +8790,9 @@
       <c r="BL71" s="113"/>
     </row>
     <row r="72" spans="2:64" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="215"/>
-      <c r="C72" s="216"/>
-      <c r="D72" s="217"/>
+      <c r="B72" s="194"/>
+      <c r="C72" s="195"/>
+      <c r="D72" s="196"/>
       <c r="E72" s="74"/>
       <c r="F72" s="73"/>
       <c r="G72" s="73"/>
@@ -8870,55 +8873,55 @@
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
-      <c r="E74" s="192" t="s">
+      <c r="E74" s="217" t="s">
         <v>2</v>
       </c>
-      <c r="F74" s="193"/>
-      <c r="G74" s="193"/>
+      <c r="F74" s="218"/>
+      <c r="G74" s="218"/>
       <c r="H74" s="64"/>
-      <c r="I74" s="192" t="s">
+      <c r="I74" s="217" t="s">
         <v>3</v>
       </c>
-      <c r="J74" s="193"/>
-      <c r="K74" s="193"/>
+      <c r="J74" s="218"/>
+      <c r="K74" s="218"/>
       <c r="L74" s="65"/>
-      <c r="M74" s="194" t="s">
+      <c r="M74" s="219" t="s">
         <v>14</v>
       </c>
-      <c r="N74" s="195"/>
-      <c r="O74" s="195"/>
+      <c r="N74" s="220"/>
+      <c r="O74" s="220"/>
       <c r="P74" s="66"/>
-      <c r="Q74" s="187" t="s">
+      <c r="Q74" s="214" t="s">
         <v>15</v>
       </c>
-      <c r="R74" s="188"/>
-      <c r="S74" s="188"/>
-      <c r="T74" s="188"/>
+      <c r="R74" s="215"/>
+      <c r="S74" s="215"/>
+      <c r="T74" s="215"/>
       <c r="U74" s="67"/>
       <c r="V74" s="135"/>
-      <c r="W74" s="188" t="s">
+      <c r="W74" s="215" t="s">
         <v>28</v>
       </c>
-      <c r="X74" s="188"/>
-      <c r="Y74" s="188"/>
+      <c r="X74" s="215"/>
+      <c r="Y74" s="215"/>
       <c r="Z74" s="68"/>
-      <c r="AA74" s="189" t="s">
+      <c r="AA74" s="180" t="s">
         <v>63</v>
       </c>
-      <c r="AB74" s="190"/>
-      <c r="AC74" s="190"/>
-      <c r="AD74" s="190"/>
-      <c r="AE74" s="190"/>
-      <c r="AF74" s="190"/>
-      <c r="AG74" s="191"/>
-      <c r="AH74" s="189" t="s">
+      <c r="AB74" s="181"/>
+      <c r="AC74" s="181"/>
+      <c r="AD74" s="181"/>
+      <c r="AE74" s="181"/>
+      <c r="AF74" s="181"/>
+      <c r="AG74" s="216"/>
+      <c r="AH74" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="AI74" s="190"/>
-      <c r="AJ74" s="190"/>
-      <c r="AK74" s="190"/>
-      <c r="AL74" s="190"/>
-      <c r="AM74" s="190"/>
+      <c r="AI74" s="181"/>
+      <c r="AJ74" s="181"/>
+      <c r="AK74" s="181"/>
+      <c r="AL74" s="181"/>
+      <c r="AM74" s="181"/>
       <c r="AN74" s="13"/>
       <c r="AO74" s="13"/>
       <c r="AP74" s="13"/>
@@ -8947,37 +8950,22 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="AH74:AM74"/>
-    <mergeCell ref="I3:L4"/>
-    <mergeCell ref="M3:P4"/>
-    <mergeCell ref="Q3:T4"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="AW3:AZ4"/>
-    <mergeCell ref="U2:AN2"/>
-    <mergeCell ref="AO2:BH2"/>
-    <mergeCell ref="Y3:AB4"/>
-    <mergeCell ref="AC3:AF4"/>
-    <mergeCell ref="AG3:AJ4"/>
-    <mergeCell ref="AK3:AN4"/>
-    <mergeCell ref="BE3:BH4"/>
-    <mergeCell ref="B71:D72"/>
-    <mergeCell ref="B69:D70"/>
-    <mergeCell ref="B67:D68"/>
-    <mergeCell ref="B65:D66"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B63:D64"/>
-    <mergeCell ref="B61:D62"/>
-    <mergeCell ref="B59:D60"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="U3:X4"/>
+    <mergeCell ref="Q74:T74"/>
+    <mergeCell ref="BA3:BD4"/>
+    <mergeCell ref="AA74:AG74"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="W74:Y74"/>
+    <mergeCell ref="I74:K74"/>
+    <mergeCell ref="M74:O74"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B49:B50"/>
     <mergeCell ref="BI2:BL2"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
@@ -8994,22 +8982,37 @@
     <mergeCell ref="AO3:AR4"/>
     <mergeCell ref="AS3:AV4"/>
     <mergeCell ref="E2:T2"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="U3:X4"/>
-    <mergeCell ref="Q74:T74"/>
-    <mergeCell ref="BA3:BD4"/>
-    <mergeCell ref="AA74:AG74"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="W74:Y74"/>
-    <mergeCell ref="I74:K74"/>
-    <mergeCell ref="M74:O74"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B71:D72"/>
+    <mergeCell ref="B69:D70"/>
+    <mergeCell ref="B67:D68"/>
+    <mergeCell ref="B65:D66"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B63:D64"/>
+    <mergeCell ref="B61:D62"/>
+    <mergeCell ref="B59:D60"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="AW3:AZ4"/>
+    <mergeCell ref="U2:AN2"/>
+    <mergeCell ref="AO2:BH2"/>
+    <mergeCell ref="Y3:AB4"/>
+    <mergeCell ref="AC3:AF4"/>
+    <mergeCell ref="AG3:AJ4"/>
+    <mergeCell ref="AK3:AN4"/>
+    <mergeCell ref="BE3:BH4"/>
+    <mergeCell ref="AH74:AM74"/>
+    <mergeCell ref="I3:L4"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="Q3:T4"/>
+    <mergeCell ref="E3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" orientation="landscape" r:id="rId1"/>
@@ -9317,21 +9320,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100501A2237DBCF164BB17DE35239A4E5F0" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="8d252ecba0bbb92ffcd60552382fd808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d5e11d0132dc5bb78ad0fb0e89938ac">
     <xsd:element name="properties">
@@ -9445,10 +9433,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9469,17 +9480,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3749D8D2-B6DE-48D8-9949-E224BC23C2D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4ABA825C-886F-4D49-8B18-F074D7C9D027}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Docs and last improvements
Closes #9
</commit_message>
<xml_diff>
--- a/docs/Zeitplan_YannickWernle.xlsx
+++ b/docs/Zeitplan_YannickWernle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\IPA\IPA\hpeilo_inventoryscript\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6315F315-4826-4F62-B20E-BAF53E2A6E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F6D63D-4632-40C9-94F4-C4777265C675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14565" yWindow="-24120" windowWidth="57840" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3595,8 +3595,8 @@
   </sheetPr>
   <dimension ref="B1:BV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AR43" sqref="AR43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AV66" sqref="AV66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,8 +3626,10 @@
     <col min="40" max="40" width="5.28515625" customWidth="1"/>
     <col min="41" max="43" width="4.28515625" customWidth="1"/>
     <col min="44" max="44" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="4.28515625" customWidth="1"/>
-    <col min="48" max="48" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.28515625" customWidth="1"/>
+    <col min="46" max="46" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="4.28515625" customWidth="1"/>
+    <col min="48" max="48" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="49" max="51" width="4.28515625" customWidth="1"/>
     <col min="52" max="52" width="5" customWidth="1"/>
     <col min="53" max="59" width="4.28515625" customWidth="1"/>
@@ -5577,7 +5579,7 @@
       </c>
       <c r="D28" s="88">
         <f>SUM(D30,D32,D34,D36,D38,D40,D42,D44,D48)</f>
-        <v>38.75</v>
+        <v>42</v>
       </c>
       <c r="E28" s="71"/>
       <c r="F28" s="69"/>
@@ -7105,7 +7107,7 @@
       </c>
       <c r="D48" s="88">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5.25</v>
       </c>
       <c r="E48" s="71"/>
       <c r="F48" s="69"/>
@@ -7150,9 +7152,15 @@
       <c r="AS48" s="146">
         <v>2</v>
       </c>
-      <c r="AT48" s="69"/>
-      <c r="AU48" s="69"/>
-      <c r="AV48" s="70"/>
+      <c r="AT48" s="140">
+        <v>0.25</v>
+      </c>
+      <c r="AU48" s="140">
+        <v>2</v>
+      </c>
+      <c r="AV48" s="163">
+        <v>1</v>
+      </c>
       <c r="AW48" s="85"/>
       <c r="AX48" s="24"/>
       <c r="AY48" s="16"/>
@@ -7253,7 +7261,7 @@
       </c>
       <c r="D50" s="89">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E50" s="74"/>
       <c r="F50" s="73"/>
@@ -7298,7 +7306,9 @@
       <c r="AS50" s="106"/>
       <c r="AT50" s="101"/>
       <c r="AU50" s="101"/>
-      <c r="AV50" s="102"/>
+      <c r="AV50" s="174">
+        <v>2</v>
+      </c>
       <c r="AW50" s="29"/>
       <c r="AX50" s="30"/>
       <c r="AY50" s="18"/>
@@ -7713,7 +7723,7 @@
       </c>
       <c r="D56" s="88">
         <f>SUM(E56:BL56)</f>
-        <v>6.95</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="E56" s="137">
         <v>1.5</v>
@@ -7778,9 +7788,13 @@
         <v>0.7</v>
       </c>
       <c r="AS56" s="109"/>
-      <c r="AT56" s="107"/>
+      <c r="AT56" s="178">
+        <v>0.75</v>
+      </c>
       <c r="AU56" s="107"/>
-      <c r="AV56" s="107"/>
+      <c r="AV56" s="178">
+        <v>1.25</v>
+      </c>
       <c r="AW56" s="29"/>
       <c r="AX56" s="30"/>
       <c r="AY56" s="107"/>
@@ -8438,9 +8452,9 @@
       <c r="AQ66" s="142"/>
       <c r="AR66" s="164"/>
       <c r="AS66" s="137"/>
-      <c r="AT66" s="18"/>
-      <c r="AU66" s="18"/>
-      <c r="AV66" s="19"/>
+      <c r="AT66" s="142"/>
+      <c r="AU66" s="142"/>
+      <c r="AV66" s="175"/>
       <c r="AW66" s="29"/>
       <c r="AX66" s="30"/>
       <c r="AY66" s="18"/>

</xml_diff>